<commit_message>
Feito todas as intruções e todo o mapeamento das instruções
</commit_message>
<xml_diff>
--- a/Files/instruction_mapping.xlsx
+++ b/Files/instruction_mapping.xlsx
@@ -504,31 +504,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B143" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Jean Carlos Klann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Pega o conteudo do registrador X e lê este valor (endereço) na memoria ram.
-Depois faz a operação ULA com o acumulador.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="N171" authorId="0" shapeId="0">
       <text>
         <r>
@@ -630,7 +605,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="69">
   <si>
     <t>Dec</t>
   </si>
@@ -779,16 +754,64 @@
     <t>RET</t>
   </si>
   <si>
-    <t>???????</t>
-  </si>
-  <si>
     <t>--------</t>
   </si>
   <si>
     <t>|</t>
   </si>
   <si>
-    <t>?</t>
+    <t>A*DRAM-&gt;A</t>
+  </si>
+  <si>
+    <t>A*A-&gt;DRAM</t>
+  </si>
+  <si>
+    <t>PUSHA</t>
+  </si>
+  <si>
+    <t>POPA</t>
+  </si>
+  <si>
+    <t>Operação/Fluxo</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>1, 6</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>HD, 2, 4</t>
+  </si>
+  <si>
+    <t>HD, 1, 3, 8</t>
+  </si>
+  <si>
+    <t>HD, 1, 3, 9</t>
+  </si>
+  <si>
+    <t>HD, 5, 3, 20</t>
+  </si>
+  <si>
+    <t>HD, HD, 5</t>
+  </si>
+  <si>
+    <t>HD, HD, 7</t>
+  </si>
+  <si>
+    <t>HD, HD, 6</t>
+  </si>
+  <si>
+    <t>HD, HD, 3</t>
+  </si>
+  <si>
+    <t>HD, HD, 4</t>
+  </si>
+  <si>
+    <t>HD, 1, 4</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1338,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1336,6 +1359,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1657,14 +1689,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:AJ171"/>
+  <dimension ref="A6:AJ171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -1698,7 +1731,13 @@
     <col min="36" max="36" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>0</v>
       </c>
@@ -1903,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>1</v>
       </c>
@@ -2008,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>2</v>
       </c>
@@ -2113,7 +2152,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>5</v>
+      </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -2221,9 +2263,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
@@ -2329,9 +2372,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -2437,9 +2481,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
@@ -2545,9 +2590,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2">
         <v>7</v>
@@ -2653,7 +2699,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>5</v>
+      </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -2761,9 +2810,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2">
         <v>9</v>
@@ -2869,9 +2919,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2">
         <v>10</v>
@@ -2977,9 +3028,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2">
         <v>11</v>
@@ -3085,9 +3137,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2">
         <v>12</v>
@@ -3193,7 +3246,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -3301,9 +3357,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2">
         <v>14</v>
@@ -3409,9 +3466,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2">
         <v>15</v>
@@ -3517,9 +3575,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2">
         <v>16</v>
@@ -3625,9 +3684,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2">
         <v>17</v>
@@ -3733,9 +3793,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2">
         <v>18</v>
@@ -3841,9 +3902,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="2">
         <v>19</v>
@@ -3949,7 +4011,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>5</v>
+      </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -4057,9 +4122,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2">
         <v>21</v>
@@ -4165,9 +4231,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2">
         <v>22</v>
@@ -4273,9 +4340,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2">
         <v>23</v>
@@ -4381,9 +4449,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2">
         <v>24</v>
@@ -4489,7 +4558,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>5</v>
+      </c>
       <c r="B32" t="s">
         <v>36</v>
       </c>
@@ -4597,9 +4669,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="2">
         <v>26</v>
@@ -4705,9 +4778,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="2">
         <v>27</v>
@@ -4813,9 +4887,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2">
         <v>28</v>
@@ -4921,9 +4996,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="2">
         <v>29</v>
@@ -5029,7 +5105,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
@@ -5137,9 +5216,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2">
         <v>31</v>
@@ -5245,7 +5325,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
       <c r="C39" s="2" t="s">
         <v>0</v>
       </c>
@@ -5345,9 +5426,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="2">
         <v>32</v>
@@ -5453,9 +5535,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2">
         <v>33</v>
@@ -5561,9 +5644,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2">
         <v>34</v>
@@ -5669,9 +5753,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="2">
         <v>35</v>
@@ -5777,9 +5862,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="2">
         <v>36</v>
@@ -5885,7 +5971,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>5</v>
+      </c>
       <c r="B45" t="s">
         <v>38</v>
       </c>
@@ -5993,9 +6082,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" s="2">
         <v>38</v>
@@ -6101,9 +6191,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="2">
         <v>39</v>
@@ -6209,9 +6300,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2">
         <v>40</v>
@@ -6317,9 +6409,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="2">
         <v>41</v>
@@ -6425,7 +6518,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="B50" t="s">
         <v>2</v>
       </c>
@@ -6533,9 +6629,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" s="2">
         <v>43</v>
@@ -6641,7 +6738,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="B52" t="s">
         <v>39</v>
       </c>
@@ -6749,9 +6849,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" s="2">
         <v>45</v>
@@ -6857,9 +6958,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" s="2">
         <v>46</v>
@@ -6965,9 +7067,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="2">
         <v>47</v>
@@ -7073,9 +7176,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2">
         <v>48</v>
@@ -7181,7 +7285,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="B57" t="s">
         <v>40</v>
       </c>
@@ -7289,9 +7396,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C58" s="2">
         <v>50</v>
@@ -7397,9 +7505,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" s="2">
         <v>51</v>
@@ -7505,9 +7614,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C60" s="2">
         <v>52</v>
@@ -7613,9 +7723,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C61" s="2">
         <v>53</v>
@@ -7721,7 +7832,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="B62" t="s">
         <v>41</v>
       </c>
@@ -7829,9 +7943,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C63" s="2">
         <v>55</v>
@@ -7937,9 +8052,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C64" s="2">
         <v>56</v>
@@ -8045,9 +8161,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="2">
         <v>57</v>
@@ -8153,9 +8270,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66" s="2">
         <v>58</v>
@@ -8261,9 +8379,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C67" s="2">
         <v>59</v>
@@ -8369,9 +8488,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C68" s="2">
         <v>60</v>
@@ -8477,7 +8597,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="B69" t="s">
         <v>42</v>
       </c>
@@ -8585,9 +8708,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
       <c r="B70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C70" s="2">
         <v>62</v>
@@ -8693,9 +8817,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C71" s="2">
         <v>63</v>
@@ -8801,7 +8926,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
       <c r="C72" s="2" t="s">
         <v>0</v>
       </c>
@@ -8901,9 +9027,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
       <c r="B73" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C73" s="2">
         <v>64</v>
@@ -9009,9 +9136,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C74" s="2">
         <v>65</v>
@@ -9117,9 +9245,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C75" s="2">
         <v>66</v>
@@ -9225,9 +9354,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C76" s="2">
         <v>67</v>
@@ -9333,9 +9463,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
       <c r="B77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C77" s="2">
         <v>68</v>
@@ -9441,9 +9572,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C78" s="2">
         <v>69</v>
@@ -9549,9 +9681,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
       <c r="B79" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C79" s="2">
         <v>70</v>
@@ -9657,9 +9790,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A80" s="8"/>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C80" s="2">
         <v>71</v>
@@ -9765,9 +9899,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C81" s="2">
         <v>72</v>
@@ -9873,7 +10008,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="B82" t="s">
         <v>43</v>
       </c>
@@ -9981,9 +10119,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A83" s="8"/>
       <c r="B83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C83" s="2">
         <v>74</v>
@@ -10089,9 +10228,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
       <c r="B84" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C84" s="2">
         <v>75</v>
@@ -10197,9 +10337,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C85" s="2">
         <v>76</v>
@@ -10305,9 +10446,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C86" s="2">
         <v>77</v>
@@ -10413,9 +10555,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C87" s="2">
         <v>78</v>
@@ -10521,9 +10664,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A88" s="8"/>
       <c r="B88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C88" s="2">
         <v>79</v>
@@ -10629,9 +10773,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A89" s="8"/>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C89" s="2">
         <v>80</v>
@@ -10737,9 +10882,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A90" s="8"/>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C90" s="2">
         <v>81</v>
@@ -10845,9 +10991,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A91" s="8"/>
       <c r="B91" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91" s="2">
         <v>82</v>
@@ -10953,9 +11100,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A92" s="8"/>
       <c r="B92" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C92" s="2">
         <v>83</v>
@@ -11061,9 +11209,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A93" s="8"/>
       <c r="B93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C93" s="2">
         <v>84</v>
@@ -11169,9 +11318,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A94" s="8"/>
       <c r="B94" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C94" s="2">
         <v>85</v>
@@ -11277,7 +11427,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="B95" t="s">
         <v>44</v>
       </c>
@@ -11385,9 +11538,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A96" s="8"/>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C96" s="2">
         <v>87</v>
@@ -11493,9 +11647,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
       <c r="B97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C97" s="2">
         <v>88</v>
@@ -11601,9 +11756,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A98" s="8"/>
       <c r="B98" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C98" s="2">
         <v>89</v>
@@ -11709,9 +11865,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A99" s="8"/>
       <c r="B99" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C99" s="2">
         <v>90</v>
@@ -11817,9 +11974,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C100" s="2">
         <v>91</v>
@@ -11925,9 +12083,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A101" s="8"/>
       <c r="B101" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C101" s="2">
         <v>92</v>
@@ -12033,9 +12192,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A102" s="8"/>
       <c r="B102" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C102" s="2">
         <v>93</v>
@@ -12141,9 +12301,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A103" s="8"/>
       <c r="B103" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C103" s="2">
         <v>94</v>
@@ -12249,9 +12410,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A104" s="8"/>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C104" s="2">
         <v>95</v>
@@ -12357,7 +12519,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A105" s="8"/>
       <c r="C105" s="2" t="s">
         <v>0</v>
       </c>
@@ -12457,9 +12620,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A106" s="8"/>
       <c r="B106" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C106" s="2">
         <v>96</v>
@@ -12565,9 +12729,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
       <c r="B107" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C107" s="2">
         <v>97</v>
@@ -12673,9 +12838,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A108" s="8"/>
       <c r="B108" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C108" s="2">
         <v>98</v>
@@ -12781,7 +12947,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="B109" t="s">
         <v>45</v>
       </c>
@@ -12889,9 +13058,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A110" s="8"/>
       <c r="B110" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C110" s="2">
         <v>100</v>
@@ -12997,9 +13167,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
       <c r="B111" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C111" s="2">
         <v>101</v>
@@ -13105,9 +13276,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
       <c r="B112" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C112" s="2">
         <v>102</v>
@@ -13213,9 +13385,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
       <c r="B113" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C113" s="2">
         <v>103</v>
@@ -13321,9 +13494,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
       <c r="B114" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C114" s="2">
         <v>104</v>
@@ -13429,9 +13603,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
       <c r="B115" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C115" s="2">
         <v>105</v>
@@ -13537,9 +13712,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A116" s="8"/>
       <c r="B116" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C116" s="2">
         <v>106</v>
@@ -13645,9 +13821,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
       <c r="B117" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C117" s="2">
         <v>107</v>
@@ -13753,9 +13930,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
       <c r="B118" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C118" s="2">
         <v>108</v>
@@ -13861,9 +14039,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
       <c r="B119" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C119" s="2">
         <v>109</v>
@@ -13969,9 +14148,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
       <c r="B120" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C120" s="2">
         <v>110</v>
@@ -14077,9 +14257,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
       <c r="B121" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C121" s="2">
         <v>111</v>
@@ -14185,9 +14366,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
       <c r="B122" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C122" s="2">
         <v>112</v>
@@ -14293,9 +14475,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
       <c r="B123" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C123" s="2">
         <v>113</v>
@@ -14401,9 +14584,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C124" s="2">
         <v>114</v>
@@ -14509,9 +14693,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A125" s="8"/>
       <c r="B125" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C125" s="2">
         <v>115</v>
@@ -14617,9 +14802,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
       <c r="B126" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C126" s="2">
         <v>116</v>
@@ -14725,9 +14911,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
       <c r="B127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C127" s="2">
         <v>117</v>
@@ -14833,9 +15020,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
       <c r="B128" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C128" s="2">
         <v>118</v>
@@ -14941,9 +15129,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
       <c r="B129" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C129" s="2">
         <v>119</v>
@@ -15049,9 +15238,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A130" s="8"/>
       <c r="B130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C130" s="2">
         <v>120</v>
@@ -15157,9 +15347,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A131" s="8"/>
       <c r="B131" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C131" s="2">
         <v>121</v>
@@ -15265,9 +15456,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A132" s="8"/>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C132" s="2">
         <v>122</v>
@@ -15373,9 +15565,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A133" s="8"/>
       <c r="B133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C133" s="2">
         <v>123</v>
@@ -15481,9 +15674,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A134" s="8"/>
       <c r="B134" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C134" s="2">
         <v>124</v>
@@ -15589,9 +15783,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A135" s="8"/>
       <c r="B135" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C135" s="2">
         <v>125</v>
@@ -15697,9 +15892,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
       <c r="B136" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C136" s="2">
         <v>126</v>
@@ -15805,7 +16001,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="B137" t="s">
         <v>48</v>
       </c>
@@ -15913,7 +16112,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
       <c r="C138" s="2" t="s">
         <v>0</v>
       </c>
@@ -16013,9 +16213,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
       <c r="B139" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C139" s="2">
         <v>128</v>
@@ -16121,9 +16322,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
       <c r="B140" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C140" s="2">
         <v>129</v>
@@ -16229,9 +16431,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
       <c r="B141" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C141" s="2">
         <v>130</v>
@@ -16337,9 +16540,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
       <c r="B142" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C142" s="2">
         <v>131</v>
@@ -16445,9 +16649,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A143" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="B143" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C143" s="2">
         <v>132</v>
@@ -16553,9 +16760,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A144" s="8"/>
       <c r="B144" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C144" s="2">
         <v>133</v>
@@ -16661,9 +16869,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A145" s="8"/>
       <c r="B145" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C145" s="2">
         <v>134</v>
@@ -16769,9 +16978,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A146" s="8"/>
       <c r="B146" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C146" s="2">
         <v>135</v>
@@ -16877,9 +17087,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A147" s="8"/>
       <c r="B147" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C147" s="2">
         <v>136</v>
@@ -16985,9 +17196,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A148" s="8"/>
       <c r="B148" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C148" s="2">
         <v>137</v>
@@ -17093,9 +17305,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A149" s="8"/>
       <c r="B149" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C149" s="2">
         <v>138</v>
@@ -17201,9 +17414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A150" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="B150" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C150" s="2">
         <v>139</v>
@@ -17309,9 +17525,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A151" s="8"/>
       <c r="B151" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C151" s="2">
         <v>140</v>
@@ -17417,9 +17634,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A152" s="8"/>
       <c r="B152" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C152" s="2">
         <v>141</v>
@@ -17525,9 +17743,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A153" s="8"/>
       <c r="B153" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C153" s="2">
         <v>142</v>
@@ -17633,9 +17852,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A154" s="8"/>
       <c r="B154" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C154" s="2">
         <v>143</v>
@@ -17741,9 +17961,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A155" s="8"/>
       <c r="B155" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C155" s="2">
         <v>144</v>
@@ -17849,7 +18070,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A156" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="B156" t="s">
         <v>46</v>
       </c>
@@ -17957,9 +18181,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A157" s="8"/>
       <c r="B157" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C157" s="2">
         <v>146</v>
@@ -18065,9 +18290,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A158" s="8"/>
       <c r="B158" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C158" s="2">
         <v>147</v>
@@ -18173,7 +18399,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A159" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="B159" t="s">
         <v>47</v>
       </c>
@@ -18281,9 +18510,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A160" s="8"/>
       <c r="B160" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C160" s="2">
         <v>149</v>
@@ -18389,9 +18619,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A161" s="8"/>
       <c r="B161" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C161" s="2">
         <v>150</v>
@@ -18497,9 +18728,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A162" s="8"/>
       <c r="B162" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C162" s="2">
         <v>151</v>
@@ -18605,9 +18837,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A163" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="B163" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C163" s="2">
         <v>152</v>
@@ -18713,9 +18948,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A164" s="8"/>
       <c r="B164" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C164" s="2">
         <v>153</v>
@@ -18821,9 +19057,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A165" s="8"/>
       <c r="B165" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C165" s="2">
         <v>154</v>
@@ -18929,9 +19166,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="B166" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C166" s="2">
         <v>155</v>
@@ -19037,9 +19277,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A167" s="8"/>
       <c r="B167" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C167" s="2">
         <v>156</v>
@@ -19145,9 +19386,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A168" s="8"/>
       <c r="B168" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C168" s="2">
         <v>157</v>
@@ -19253,9 +19495,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A169" s="8"/>
       <c r="B169" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C169" s="2">
         <v>158</v>
@@ -19361,9 +19604,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A170" s="9"/>
       <c r="B170" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C170" s="2">
         <v>159</v>
@@ -19469,7 +19713,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A171" s="9"/>
       <c r="C171" s="2" t="s">
         <v>0</v>
       </c>
@@ -19570,6 +19815,30 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A163:A165"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="A109:A136"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A143:A149"/>
+    <mergeCell ref="A150:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A159:A162"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="A69:A81"/>
+    <mergeCell ref="A82:A94"/>
+    <mergeCell ref="A95:A108"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Várias instruçõs funcionando. JMP ainda não funcionando (já guarda o valor nas memorias ram, pore´m não os envia corretamente para a ROM). Arrumado erros na memoria ram e no circuito.
</commit_message>
<xml_diff>
--- a/Files/instruction_mapping.xlsx
+++ b/Files/instruction_mapping.xlsx
@@ -967,7 +967,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1177,6 +1177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1338,7 +1344,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1360,10 +1366,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1691,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:AJ171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1741,7 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="s">
@@ -2153,7 +2162,7 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="11">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -2264,7 +2273,7 @@
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -2373,7 +2382,7 @@
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -2482,7 +2491,7 @@
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" t="s">
         <v>50</v>
       </c>
@@ -2591,7 +2600,7 @@
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -2700,7 +2709,7 @@
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="11">
         <v>5</v>
       </c>
       <c r="B15" t="s">
@@ -2811,7 +2820,7 @@
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -2920,7 +2929,7 @@
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" t="s">
         <v>50</v>
       </c>
@@ -3029,7 +3038,7 @@
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -3138,7 +3147,7 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="11"/>
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -3247,7 +3256,7 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
@@ -3358,7 +3367,7 @@
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="11"/>
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -3467,7 +3476,7 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="11"/>
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -3576,7 +3585,7 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="11"/>
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -3685,7 +3694,7 @@
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -3794,7 +3803,7 @@
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -3903,7 +3912,7 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="11"/>
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -4012,7 +4021,7 @@
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="11">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -4123,7 +4132,7 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="11"/>
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -4232,7 +4241,7 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="11"/>
       <c r="B29" t="s">
         <v>50</v>
       </c>
@@ -4341,7 +4350,7 @@
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="11"/>
       <c r="B30" t="s">
         <v>50</v>
       </c>
@@ -4450,7 +4459,7 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
       <c r="B31" t="s">
         <v>50</v>
       </c>
@@ -4559,7 +4568,7 @@
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="11">
         <v>5</v>
       </c>
       <c r="B32" t="s">
@@ -4670,7 +4679,7 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="11"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -4779,7 +4788,7 @@
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="11"/>
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -4888,7 +4897,7 @@
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="11"/>
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -4997,7 +5006,7 @@
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="11"/>
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -5106,7 +5115,7 @@
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
@@ -5217,7 +5226,7 @@
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="11"/>
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -5326,7 +5335,7 @@
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="11"/>
       <c r="C39" s="2" t="s">
         <v>0</v>
       </c>
@@ -5427,7 +5436,7 @@
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="11"/>
       <c r="B40" t="s">
         <v>50</v>
       </c>
@@ -5536,7 +5545,7 @@
       </c>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="11"/>
       <c r="B41" t="s">
         <v>50</v>
       </c>
@@ -5645,7 +5654,7 @@
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="11"/>
       <c r="B42" t="s">
         <v>50</v>
       </c>
@@ -5754,7 +5763,7 @@
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="11"/>
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -5863,7 +5872,7 @@
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="11"/>
       <c r="B44" t="s">
         <v>50</v>
       </c>
@@ -5972,7 +5981,7 @@
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+      <c r="A45" s="11">
         <v>5</v>
       </c>
       <c r="B45" t="s">
@@ -6083,7 +6092,7 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="11"/>
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -6192,7 +6201,7 @@
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+      <c r="A47" s="11"/>
       <c r="B47" t="s">
         <v>50</v>
       </c>
@@ -6301,7 +6310,7 @@
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
+      <c r="A48" s="11"/>
       <c r="B48" t="s">
         <v>50</v>
       </c>
@@ -6410,7 +6419,7 @@
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="11"/>
       <c r="B49" t="s">
         <v>50</v>
       </c>
@@ -6519,7 +6528,7 @@
       </c>
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B50" t="s">
@@ -6630,7 +6639,7 @@
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="11"/>
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -6739,7 +6748,7 @@
       </c>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B52" t="s">
@@ -6850,7 +6859,7 @@
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="11"/>
       <c r="B53" t="s">
         <v>50</v>
       </c>
@@ -6959,7 +6968,7 @@
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="11"/>
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -7068,7 +7077,7 @@
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="11"/>
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -7177,7 +7186,7 @@
       </c>
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="11"/>
       <c r="B56" t="s">
         <v>50</v>
       </c>
@@ -7286,7 +7295,7 @@
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B57" t="s">
@@ -7397,7 +7406,7 @@
       </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
+      <c r="A58" s="11"/>
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -7506,7 +7515,7 @@
       </c>
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
+      <c r="A59" s="11"/>
       <c r="B59" t="s">
         <v>50</v>
       </c>
@@ -7615,7 +7624,7 @@
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
+      <c r="A60" s="11"/>
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -7724,7 +7733,7 @@
       </c>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
+      <c r="A61" s="11"/>
       <c r="B61" t="s">
         <v>50</v>
       </c>
@@ -7833,7 +7842,7 @@
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B62" t="s">
@@ -7944,7 +7953,7 @@
       </c>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
+      <c r="A63" s="11"/>
       <c r="B63" t="s">
         <v>50</v>
       </c>
@@ -8053,7 +8062,7 @@
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
+      <c r="A64" s="11"/>
       <c r="B64" t="s">
         <v>50</v>
       </c>
@@ -8162,7 +8171,7 @@
       </c>
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
+      <c r="A65" s="11"/>
       <c r="B65" t="s">
         <v>50</v>
       </c>
@@ -8271,7 +8280,7 @@
       </c>
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
+      <c r="A66" s="11"/>
       <c r="B66" t="s">
         <v>50</v>
       </c>
@@ -8380,7 +8389,7 @@
       </c>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
+      <c r="A67" s="11"/>
       <c r="B67" t="s">
         <v>50</v>
       </c>
@@ -8489,7 +8498,7 @@
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
+      <c r="A68" s="11"/>
       <c r="B68" t="s">
         <v>50</v>
       </c>
@@ -8598,7 +8607,7 @@
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B69" t="s">
@@ -8709,7 +8718,7 @@
       </c>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
+      <c r="A70" s="11"/>
       <c r="B70" t="s">
         <v>50</v>
       </c>
@@ -8818,7 +8827,7 @@
       </c>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
+      <c r="A71" s="11"/>
       <c r="B71" t="s">
         <v>50</v>
       </c>
@@ -8927,7 +8936,7 @@
       </c>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
+      <c r="A72" s="11"/>
       <c r="C72" s="2" t="s">
         <v>0</v>
       </c>
@@ -9028,7 +9037,7 @@
       </c>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
+      <c r="A73" s="11"/>
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -9137,7 +9146,7 @@
       </c>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
+      <c r="A74" s="11"/>
       <c r="B74" t="s">
         <v>50</v>
       </c>
@@ -9246,7 +9255,7 @@
       </c>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
+      <c r="A75" s="11"/>
       <c r="B75" t="s">
         <v>50</v>
       </c>
@@ -9355,7 +9364,7 @@
       </c>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
+      <c r="A76" s="11"/>
       <c r="B76" t="s">
         <v>50</v>
       </c>
@@ -9464,7 +9473,7 @@
       </c>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
+      <c r="A77" s="11"/>
       <c r="B77" t="s">
         <v>50</v>
       </c>
@@ -9573,7 +9582,7 @@
       </c>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
+      <c r="A78" s="11"/>
       <c r="B78" t="s">
         <v>50</v>
       </c>
@@ -9593,8 +9602,8 @@
       <c r="G78" s="4">
         <v>0</v>
       </c>
-      <c r="H78" s="4">
-        <v>0</v>
+      <c r="H78" s="10">
+        <v>1</v>
       </c>
       <c r="I78" s="3">
         <v>1</v>
@@ -9682,7 +9691,7 @@
       </c>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
+      <c r="A79" s="11"/>
       <c r="B79" t="s">
         <v>50</v>
       </c>
@@ -9791,7 +9800,7 @@
       </c>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
+      <c r="A80" s="11"/>
       <c r="B80" t="s">
         <v>50</v>
       </c>
@@ -9811,8 +9820,8 @@
       <c r="G80" s="4">
         <v>0</v>
       </c>
-      <c r="H80" s="4">
-        <v>0</v>
+      <c r="H80" s="10">
+        <v>1</v>
       </c>
       <c r="I80" s="3">
         <v>0</v>
@@ -9900,7 +9909,7 @@
       </c>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A81" s="8"/>
+      <c r="A81" s="11"/>
       <c r="B81" t="s">
         <v>50</v>
       </c>
@@ -10009,7 +10018,7 @@
       </c>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B82" t="s">
@@ -10120,7 +10129,7 @@
       </c>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
+      <c r="A83" s="11"/>
       <c r="B83" t="s">
         <v>50</v>
       </c>
@@ -10229,7 +10238,7 @@
       </c>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
+      <c r="A84" s="11"/>
       <c r="B84" t="s">
         <v>50</v>
       </c>
@@ -10338,7 +10347,7 @@
       </c>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
+      <c r="A85" s="11"/>
       <c r="B85" t="s">
         <v>50</v>
       </c>
@@ -10447,7 +10456,7 @@
       </c>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
+      <c r="A86" s="11"/>
       <c r="B86" t="s">
         <v>50</v>
       </c>
@@ -10556,7 +10565,7 @@
       </c>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A87" s="8"/>
+      <c r="A87" s="11"/>
       <c r="B87" t="s">
         <v>50</v>
       </c>
@@ -10665,7 +10674,7 @@
       </c>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A88" s="8"/>
+      <c r="A88" s="11"/>
       <c r="B88" t="s">
         <v>50</v>
       </c>
@@ -10774,7 +10783,7 @@
       </c>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A89" s="8"/>
+      <c r="A89" s="11"/>
       <c r="B89" t="s">
         <v>50</v>
       </c>
@@ -10883,7 +10892,7 @@
       </c>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A90" s="8"/>
+      <c r="A90" s="11"/>
       <c r="B90" t="s">
         <v>50</v>
       </c>
@@ -10992,7 +11001,7 @@
       </c>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A91" s="8"/>
+      <c r="A91" s="11"/>
       <c r="B91" t="s">
         <v>50</v>
       </c>
@@ -11012,8 +11021,8 @@
       <c r="G91" s="4">
         <v>0</v>
       </c>
-      <c r="H91" s="4">
-        <v>0</v>
+      <c r="H91" s="10">
+        <v>1</v>
       </c>
       <c r="I91" s="3">
         <v>1</v>
@@ -11101,7 +11110,7 @@
       </c>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A92" s="8"/>
+      <c r="A92" s="11"/>
       <c r="B92" t="s">
         <v>50</v>
       </c>
@@ -11210,7 +11219,7 @@
       </c>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
+      <c r="A93" s="11"/>
       <c r="B93" t="s">
         <v>50</v>
       </c>
@@ -11230,8 +11239,8 @@
       <c r="G93" s="4">
         <v>0</v>
       </c>
-      <c r="H93" s="4">
-        <v>0</v>
+      <c r="H93" s="10">
+        <v>1</v>
       </c>
       <c r="I93" s="3">
         <v>0</v>
@@ -11319,7 +11328,7 @@
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="8"/>
+      <c r="A94" s="11"/>
       <c r="B94" t="s">
         <v>50</v>
       </c>
@@ -11428,7 +11437,7 @@
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B95" t="s">
@@ -11539,7 +11548,7 @@
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A96" s="8"/>
+      <c r="A96" s="11"/>
       <c r="B96" t="s">
         <v>50</v>
       </c>
@@ -11648,7 +11657,7 @@
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
+      <c r="A97" s="11"/>
       <c r="B97" t="s">
         <v>50</v>
       </c>
@@ -11757,7 +11766,7 @@
       </c>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
+      <c r="A98" s="11"/>
       <c r="B98" t="s">
         <v>50</v>
       </c>
@@ -11866,7 +11875,7 @@
       </c>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A99" s="8"/>
+      <c r="A99" s="11"/>
       <c r="B99" t="s">
         <v>50</v>
       </c>
@@ -11975,7 +11984,7 @@
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A100" s="8"/>
+      <c r="A100" s="11"/>
       <c r="B100" t="s">
         <v>50</v>
       </c>
@@ -12084,7 +12093,7 @@
       </c>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A101" s="8"/>
+      <c r="A101" s="11"/>
       <c r="B101" t="s">
         <v>50</v>
       </c>
@@ -12193,7 +12202,7 @@
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A102" s="8"/>
+      <c r="A102" s="11"/>
       <c r="B102" t="s">
         <v>50</v>
       </c>
@@ -12302,7 +12311,7 @@
       </c>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A103" s="8"/>
+      <c r="A103" s="11"/>
       <c r="B103" t="s">
         <v>50</v>
       </c>
@@ -12411,7 +12420,7 @@
       </c>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A104" s="8"/>
+      <c r="A104" s="11"/>
       <c r="B104" t="s">
         <v>50</v>
       </c>
@@ -12431,8 +12440,8 @@
       <c r="G104" s="4">
         <v>0</v>
       </c>
-      <c r="H104" s="4">
-        <v>0</v>
+      <c r="H104" s="10">
+        <v>1</v>
       </c>
       <c r="I104" s="3">
         <v>1</v>
@@ -12520,7 +12529,7 @@
       </c>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
+      <c r="A105" s="11"/>
       <c r="C105" s="2" t="s">
         <v>0</v>
       </c>
@@ -12621,7 +12630,7 @@
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
+      <c r="A106" s="11"/>
       <c r="B106" t="s">
         <v>50</v>
       </c>
@@ -12730,7 +12739,7 @@
       </c>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
+      <c r="A107" s="11"/>
       <c r="B107" t="s">
         <v>50</v>
       </c>
@@ -12750,8 +12759,8 @@
       <c r="G107" s="4">
         <v>0</v>
       </c>
-      <c r="H107" s="4">
-        <v>0</v>
+      <c r="H107" s="10">
+        <v>1</v>
       </c>
       <c r="I107" s="3">
         <v>0</v>
@@ -12839,7 +12848,7 @@
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A108" s="8"/>
+      <c r="A108" s="11"/>
       <c r="B108" t="s">
         <v>50</v>
       </c>
@@ -12948,7 +12957,7 @@
       </c>
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B109" t="s">
@@ -13059,7 +13068,7 @@
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A110" s="8"/>
+      <c r="A110" s="11"/>
       <c r="B110" t="s">
         <v>50</v>
       </c>
@@ -13168,7 +13177,7 @@
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
+      <c r="A111" s="11"/>
       <c r="B111" t="s">
         <v>50</v>
       </c>
@@ -13277,7 +13286,7 @@
       </c>
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A112" s="8"/>
+      <c r="A112" s="11"/>
       <c r="B112" t="s">
         <v>50</v>
       </c>
@@ -13386,7 +13395,7 @@
       </c>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
+      <c r="A113" s="11"/>
       <c r="B113" t="s">
         <v>50</v>
       </c>
@@ -13495,7 +13504,7 @@
       </c>
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
+      <c r="A114" s="11"/>
       <c r="B114" t="s">
         <v>50</v>
       </c>
@@ -13604,7 +13613,7 @@
       </c>
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
+      <c r="A115" s="11"/>
       <c r="B115" t="s">
         <v>50</v>
       </c>
@@ -13713,7 +13722,7 @@
       </c>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
+      <c r="A116" s="11"/>
       <c r="B116" t="s">
         <v>50</v>
       </c>
@@ -13822,7 +13831,7 @@
       </c>
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
+      <c r="A117" s="11"/>
       <c r="B117" t="s">
         <v>50</v>
       </c>
@@ -13931,7 +13940,7 @@
       </c>
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
+      <c r="A118" s="11"/>
       <c r="B118" t="s">
         <v>50</v>
       </c>
@@ -14040,7 +14049,7 @@
       </c>
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
+      <c r="A119" s="11"/>
       <c r="B119" t="s">
         <v>50</v>
       </c>
@@ -14149,7 +14158,7 @@
       </c>
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
+      <c r="A120" s="11"/>
       <c r="B120" t="s">
         <v>50</v>
       </c>
@@ -14258,7 +14267,7 @@
       </c>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A121" s="8"/>
+      <c r="A121" s="11"/>
       <c r="B121" t="s">
         <v>50</v>
       </c>
@@ -14367,7 +14376,7 @@
       </c>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
+      <c r="A122" s="11"/>
       <c r="B122" t="s">
         <v>50</v>
       </c>
@@ -14476,7 +14485,7 @@
       </c>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A123" s="8"/>
+      <c r="A123" s="11"/>
       <c r="B123" t="s">
         <v>50</v>
       </c>
@@ -14585,7 +14594,7 @@
       </c>
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A124" s="8"/>
+      <c r="A124" s="11"/>
       <c r="B124" t="s">
         <v>50</v>
       </c>
@@ -14694,7 +14703,7 @@
       </c>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A125" s="8"/>
+      <c r="A125" s="11"/>
       <c r="B125" t="s">
         <v>50</v>
       </c>
@@ -14803,7 +14812,7 @@
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A126" s="8"/>
+      <c r="A126" s="11"/>
       <c r="B126" t="s">
         <v>50</v>
       </c>
@@ -14912,7 +14921,7 @@
       </c>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A127" s="8"/>
+      <c r="A127" s="11"/>
       <c r="B127" t="s">
         <v>50</v>
       </c>
@@ -15021,7 +15030,7 @@
       </c>
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
+      <c r="A128" s="11"/>
       <c r="B128" t="s">
         <v>50</v>
       </c>
@@ -15130,7 +15139,7 @@
       </c>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A129" s="8"/>
+      <c r="A129" s="11"/>
       <c r="B129" t="s">
         <v>50</v>
       </c>
@@ -15239,7 +15248,7 @@
       </c>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A130" s="8"/>
+      <c r="A130" s="11"/>
       <c r="B130" t="s">
         <v>50</v>
       </c>
@@ -15348,7 +15357,7 @@
       </c>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A131" s="8"/>
+      <c r="A131" s="11"/>
       <c r="B131" t="s">
         <v>50</v>
       </c>
@@ -15457,7 +15466,7 @@
       </c>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
+      <c r="A132" s="11"/>
       <c r="B132" t="s">
         <v>50</v>
       </c>
@@ -15566,7 +15575,7 @@
       </c>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A133" s="8"/>
+      <c r="A133" s="11"/>
       <c r="B133" t="s">
         <v>50</v>
       </c>
@@ -15586,8 +15595,8 @@
       <c r="G133" s="4">
         <v>0</v>
       </c>
-      <c r="H133" s="4">
-        <v>0</v>
+      <c r="H133" s="10">
+        <v>1</v>
       </c>
       <c r="I133" s="3">
         <v>1</v>
@@ -15675,7 +15684,7 @@
       </c>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A134" s="8"/>
+      <c r="A134" s="11"/>
       <c r="B134" t="s">
         <v>50</v>
       </c>
@@ -15784,7 +15793,7 @@
       </c>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A135" s="8"/>
+      <c r="A135" s="11"/>
       <c r="B135" t="s">
         <v>50</v>
       </c>
@@ -15804,8 +15813,8 @@
       <c r="G135" s="4">
         <v>0</v>
       </c>
-      <c r="H135" s="4">
-        <v>0</v>
+      <c r="H135" s="10">
+        <v>1</v>
       </c>
       <c r="I135" s="3">
         <v>0</v>
@@ -15893,7 +15902,7 @@
       </c>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
+      <c r="A136" s="11"/>
       <c r="B136" t="s">
         <v>50</v>
       </c>
@@ -16002,7 +16011,7 @@
       </c>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
+      <c r="A137" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B137" t="s">
@@ -16113,7 +16122,7 @@
       </c>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A138" s="8"/>
+      <c r="A138" s="11"/>
       <c r="C138" s="2" t="s">
         <v>0</v>
       </c>
@@ -16214,7 +16223,7 @@
       </c>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A139" s="8"/>
+      <c r="A139" s="11"/>
       <c r="B139" t="s">
         <v>50</v>
       </c>
@@ -16234,8 +16243,8 @@
       <c r="G139" s="4">
         <v>0</v>
       </c>
-      <c r="H139" s="4">
-        <v>0</v>
+      <c r="H139" s="10">
+        <v>1</v>
       </c>
       <c r="I139" s="3">
         <v>1</v>
@@ -16323,7 +16332,7 @@
       </c>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A140" s="8"/>
+      <c r="A140" s="11"/>
       <c r="B140" t="s">
         <v>50</v>
       </c>
@@ -16432,7 +16441,7 @@
       </c>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A141" s="8"/>
+      <c r="A141" s="11"/>
       <c r="B141" t="s">
         <v>50</v>
       </c>
@@ -16452,8 +16461,8 @@
       <c r="G141" s="4">
         <v>0</v>
       </c>
-      <c r="H141" s="4">
-        <v>0</v>
+      <c r="H141" s="10">
+        <v>1</v>
       </c>
       <c r="I141" s="3">
         <v>0</v>
@@ -16541,7 +16550,7 @@
       </c>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A142" s="8"/>
+      <c r="A142" s="11"/>
       <c r="B142" t="s">
         <v>50</v>
       </c>
@@ -16650,7 +16659,7 @@
       </c>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A143" s="8" t="s">
+      <c r="A143" s="11" t="s">
         <v>64</v>
       </c>
       <c r="B143" t="s">
@@ -16761,7 +16770,7 @@
       </c>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A144" s="8"/>
+      <c r="A144" s="11"/>
       <c r="B144" t="s">
         <v>50</v>
       </c>
@@ -16870,7 +16879,7 @@
       </c>
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A145" s="8"/>
+      <c r="A145" s="11"/>
       <c r="B145" t="s">
         <v>50</v>
       </c>
@@ -16979,7 +16988,7 @@
       </c>
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A146" s="8"/>
+      <c r="A146" s="11"/>
       <c r="B146" t="s">
         <v>50</v>
       </c>
@@ -17088,7 +17097,7 @@
       </c>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A147" s="8"/>
+      <c r="A147" s="11"/>
       <c r="B147" t="s">
         <v>50</v>
       </c>
@@ -17197,7 +17206,7 @@
       </c>
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A148" s="8"/>
+      <c r="A148" s="11"/>
       <c r="B148" t="s">
         <v>50</v>
       </c>
@@ -17306,7 +17315,7 @@
       </c>
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A149" s="8"/>
+      <c r="A149" s="11"/>
       <c r="B149" t="s">
         <v>50</v>
       </c>
@@ -17415,7 +17424,7 @@
       </c>
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
+      <c r="A150" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B150" t="s">
@@ -17526,7 +17535,7 @@
       </c>
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A151" s="8"/>
+      <c r="A151" s="11"/>
       <c r="B151" t="s">
         <v>50</v>
       </c>
@@ -17635,7 +17644,7 @@
       </c>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A152" s="8"/>
+      <c r="A152" s="11"/>
       <c r="B152" t="s">
         <v>50</v>
       </c>
@@ -17744,7 +17753,7 @@
       </c>
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A153" s="8"/>
+      <c r="A153" s="11"/>
       <c r="B153" t="s">
         <v>50</v>
       </c>
@@ -17853,7 +17862,7 @@
       </c>
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A154" s="8"/>
+      <c r="A154" s="11"/>
       <c r="B154" t="s">
         <v>50</v>
       </c>
@@ -17962,7 +17971,7 @@
       </c>
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A155" s="8"/>
+      <c r="A155" s="11"/>
       <c r="B155" t="s">
         <v>50</v>
       </c>
@@ -18071,7 +18080,7 @@
       </c>
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A156" s="8" t="s">
+      <c r="A156" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B156" t="s">
@@ -18182,7 +18191,7 @@
       </c>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A157" s="8"/>
+      <c r="A157" s="11"/>
       <c r="B157" t="s">
         <v>50</v>
       </c>
@@ -18291,7 +18300,7 @@
       </c>
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A158" s="8"/>
+      <c r="A158" s="11"/>
       <c r="B158" t="s">
         <v>50</v>
       </c>
@@ -18400,7 +18409,7 @@
       </c>
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A159" s="8" t="s">
+      <c r="A159" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B159" t="s">
@@ -18511,7 +18520,7 @@
       </c>
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A160" s="8"/>
+      <c r="A160" s="11"/>
       <c r="B160" t="s">
         <v>50</v>
       </c>
@@ -18620,7 +18629,7 @@
       </c>
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A161" s="8"/>
+      <c r="A161" s="11"/>
       <c r="B161" t="s">
         <v>50</v>
       </c>
@@ -18729,7 +18738,7 @@
       </c>
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A162" s="8"/>
+      <c r="A162" s="11"/>
       <c r="B162" t="s">
         <v>50</v>
       </c>
@@ -18838,7 +18847,7 @@
       </c>
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A163" s="8" t="s">
+      <c r="A163" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B163" t="s">
@@ -18949,7 +18958,7 @@
       </c>
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A164" s="8"/>
+      <c r="A164" s="11"/>
       <c r="B164" t="s">
         <v>50</v>
       </c>
@@ -19058,7 +19067,7 @@
       </c>
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A165" s="8"/>
+      <c r="A165" s="11"/>
       <c r="B165" t="s">
         <v>50</v>
       </c>
@@ -19167,7 +19176,7 @@
       </c>
     </row>
     <row r="166" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A166" s="8" t="s">
+      <c r="A166" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B166" t="s">
@@ -19278,7 +19287,7 @@
       </c>
     </row>
     <row r="167" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A167" s="8"/>
+      <c r="A167" s="11"/>
       <c r="B167" t="s">
         <v>50</v>
       </c>
@@ -19387,7 +19396,7 @@
       </c>
     </row>
     <row r="168" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A168" s="8"/>
+      <c r="A168" s="11"/>
       <c r="B168" t="s">
         <v>50</v>
       </c>
@@ -19496,7 +19505,7 @@
       </c>
     </row>
     <row r="169" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A169" s="8"/>
+      <c r="A169" s="11"/>
       <c r="B169" t="s">
         <v>50</v>
       </c>
@@ -19605,7 +19614,7 @@
       </c>
     </row>
     <row r="170" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A170" s="9"/>
+      <c r="A170" s="8"/>
       <c r="B170" s="7" t="s">
         <v>49</v>
       </c>
@@ -19714,7 +19723,7 @@
       </c>
     </row>
     <row r="171" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A171" s="9"/>
+      <c r="A171" s="8"/>
       <c r="C171" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Quase terminado. Apenas os JMPZ e JMPC não estão funcionando. (JMPC não testado). Feito a tela sobre e ajuda.
</commit_message>
<xml_diff>
--- a/Files/instruction_mapping.xlsx
+++ b/Files/instruction_mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M3PlusMicrocontrollerSimulator\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\M3PlusMicrocontroller\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="instruction_mapping" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="71">
   <si>
     <t>Dec</t>
   </si>
@@ -1015,6 +1015,12 @@
   </si>
   <si>
     <t>HD, 1, 4</t>
+  </si>
+  <si>
+    <t>Colunas1</t>
+  </si>
+  <si>
+    <t>Colunas2</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1583,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1628,7 +1634,332 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1639,6 +1970,52 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B6:AJ166" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B6:AJ166"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Operação/Fluxo"/>
+    <tableColumn id="2" name="Dec" dataDxfId="35"/>
+    <tableColumn id="3" name="Hex" dataDxfId="34">
+      <calculatedColumnFormula>DEC2HEX(C7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="SPIncDec" dataDxfId="33"/>
+    <tableColumn id="5" name="SP clock" dataDxfId="32"/>
+    <tableColumn id="6" name="DIRClock" dataDxfId="31"/>
+    <tableColumn id="7" name="SelDataPC" dataDxfId="30"/>
+    <tableColumn id="8" name="Clock PCL" dataDxfId="29"/>
+    <tableColumn id="9" name="Clock PCH" dataDxfId="28"/>
+    <tableColumn id="10" name="PCL Bus" dataDxfId="27"/>
+    <tableColumn id="11" name="PCH Bus" dataDxfId="26"/>
+    <tableColumn id="12" name="ROM cs" dataDxfId="25"/>
+    <tableColumn id="13" name="ROM rd" dataDxfId="24"/>
+    <tableColumn id="14" name="HD clock" dataDxfId="23"/>
+    <tableColumn id="15" name="SelRI" dataDxfId="22"/>
+    <tableColumn id="16" name="RIClock" dataDxfId="21"/>
+    <tableColumn id="17" name="CresZ" dataDxfId="20"/>
+    <tableColumn id="18" name="CresC" dataDxfId="19"/>
+    <tableColumn id="19" name="Cres" dataDxfId="18"/>
+    <tableColumn id="20" name="Colunas1" dataDxfId="17"/>
+    <tableColumn id="21" name="Colunas2" dataDxfId="16"/>
+    <tableColumn id="22" name="HD res" dataDxfId="15"/>
+    <tableColumn id="23" name="HD" dataDxfId="14"/>
+    <tableColumn id="24" name="Out clock" dataDxfId="13"/>
+    <tableColumn id="25" name="IN Bus" dataDxfId="12"/>
+    <tableColumn id="26" name="RAM cs" dataDxfId="11"/>
+    <tableColumn id="27" name="Ram wr" dataDxfId="10"/>
+    <tableColumn id="28" name="RAM rd" dataDxfId="9"/>
+    <tableColumn id="29" name="Reg Clock" dataDxfId="8"/>
+    <tableColumn id="30" name="Reg Bus" dataDxfId="7"/>
+    <tableColumn id="31" name="AC Clock" dataDxfId="6"/>
+    <tableColumn id="32" name="AC Bus" dataDxfId="5"/>
+    <tableColumn id="33" name="BUF Clock" dataDxfId="4"/>
+    <tableColumn id="34" name="ULA Bus" dataDxfId="3"/>
+    <tableColumn id="35" name="Sel SP" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2368,7 +2745,7 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -2479,7 +2856,7 @@
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -2588,7 +2965,7 @@
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -2697,7 +3074,7 @@
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>50</v>
       </c>
@@ -2806,7 +3183,7 @@
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -2915,7 +3292,7 @@
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="12">
         <v>5</v>
       </c>
       <c r="B15" t="s">
@@ -3026,7 +3403,7 @@
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -3135,7 +3512,7 @@
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" t="s">
         <v>50</v>
       </c>
@@ -3244,7 +3621,7 @@
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -3353,7 +3730,7 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -3462,7 +3839,7 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
@@ -3573,7 +3950,7 @@
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -3682,7 +4059,7 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -3791,7 +4168,7 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -3900,7 +4277,7 @@
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -4009,7 +4386,7 @@
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -4118,7 +4495,7 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -4227,7 +4604,7 @@
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="12">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -4338,7 +4715,7 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -4447,7 +4824,7 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>50</v>
       </c>
@@ -4556,7 +4933,7 @@
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" t="s">
         <v>50</v>
       </c>
@@ -4665,7 +5042,7 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>50</v>
       </c>
@@ -4774,7 +5151,7 @@
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="12">
         <v>5</v>
       </c>
       <c r="B32" t="s">
@@ -4885,7 +5262,7 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -4994,7 +5371,7 @@
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -5103,7 +5480,7 @@
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -5212,7 +5589,7 @@
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -5321,7 +5698,7 @@
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
@@ -5432,7 +5809,7 @@
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -5541,7 +5918,7 @@
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="C39" s="2" t="s">
         <v>0</v>
       </c>
@@ -5642,7 +6019,7 @@
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="12"/>
       <c r="B40" t="s">
         <v>50</v>
       </c>
@@ -5751,7 +6128,7 @@
       </c>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="12"/>
       <c r="B41" t="s">
         <v>50</v>
       </c>
@@ -5860,7 +6237,7 @@
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="12"/>
       <c r="B42" t="s">
         <v>50</v>
       </c>
@@ -5969,7 +6346,7 @@
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="12"/>
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -6078,7 +6455,7 @@
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="12"/>
       <c r="B44" t="s">
         <v>50</v>
       </c>
@@ -6187,7 +6564,7 @@
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="A45" s="12">
         <v>5</v>
       </c>
       <c r="B45" t="s">
@@ -6298,7 +6675,7 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -6407,7 +6784,7 @@
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>50</v>
       </c>
@@ -6516,7 +6893,7 @@
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+      <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>50</v>
       </c>
@@ -6625,7 +7002,7 @@
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+      <c r="A49" s="12"/>
       <c r="B49" t="s">
         <v>50</v>
       </c>
@@ -6734,7 +7111,7 @@
       </c>
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B50" t="s">
@@ -6845,7 +7222,7 @@
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+      <c r="A51" s="12"/>
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -6954,7 +7331,7 @@
       </c>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B52" t="s">
@@ -7065,7 +7442,7 @@
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
+      <c r="A53" s="12"/>
       <c r="B53" t="s">
         <v>50</v>
       </c>
@@ -7174,7 +7551,7 @@
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
+      <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -7283,7 +7660,7 @@
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+      <c r="A55" s="12"/>
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -7392,7 +7769,7 @@
       </c>
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
+      <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>50</v>
       </c>
@@ -7501,7 +7878,7 @@
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B57" t="s">
@@ -7612,7 +7989,7 @@
       </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
+      <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -7721,7 +8098,7 @@
       </c>
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
+      <c r="A59" s="12"/>
       <c r="B59" t="s">
         <v>50</v>
       </c>
@@ -7830,7 +8207,7 @@
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+      <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -7939,7 +8316,7 @@
       </c>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
+      <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>50</v>
       </c>
@@ -8048,7 +8425,7 @@
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B62" t="s">
@@ -8159,7 +8536,7 @@
       </c>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
+      <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>50</v>
       </c>
@@ -8268,7 +8645,7 @@
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
+      <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>50</v>
       </c>
@@ -8377,7 +8754,7 @@
       </c>
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
+      <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>50</v>
       </c>
@@ -8486,7 +8863,7 @@
       </c>
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
+      <c r="A66" s="12"/>
       <c r="B66" t="s">
         <v>50</v>
       </c>
@@ -8595,7 +8972,7 @@
       </c>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+      <c r="A67" s="12"/>
       <c r="B67" t="s">
         <v>50</v>
       </c>
@@ -8704,7 +9081,7 @@
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
+      <c r="A68" s="12"/>
       <c r="B68" t="s">
         <v>50</v>
       </c>
@@ -8813,7 +9190,7 @@
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B69" t="s">
@@ -8924,7 +9301,7 @@
       </c>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
+      <c r="A70" s="12"/>
       <c r="B70" t="s">
         <v>50</v>
       </c>
@@ -9033,7 +9410,7 @@
       </c>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
+      <c r="A71" s="12"/>
       <c r="B71" t="s">
         <v>50</v>
       </c>
@@ -9142,7 +9519,7 @@
       </c>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+      <c r="A72" s="12"/>
       <c r="C72" s="2" t="s">
         <v>0</v>
       </c>
@@ -9243,7 +9620,7 @@
       </c>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
+      <c r="A73" s="12"/>
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -9352,7 +9729,7 @@
       </c>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
+      <c r="A74" s="12"/>
       <c r="B74" t="s">
         <v>50</v>
       </c>
@@ -9461,7 +9838,7 @@
       </c>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
+      <c r="A75" s="12"/>
       <c r="B75" t="s">
         <v>50</v>
       </c>
@@ -9570,7 +9947,7 @@
       </c>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+      <c r="A76" s="12"/>
       <c r="B76" t="s">
         <v>50</v>
       </c>
@@ -9679,7 +10056,7 @@
       </c>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+      <c r="A77" s="12"/>
       <c r="B77" t="s">
         <v>50</v>
       </c>
@@ -9788,11 +10165,11 @@
       </c>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+      <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>50</v>
       </c>
-      <c r="C78" s="12">
+      <c r="C78" s="11">
         <v>69</v>
       </c>
       <c r="D78" s="2" t="str">
@@ -9897,7 +10274,7 @@
       </c>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
+      <c r="A79" s="12"/>
       <c r="B79" t="s">
         <v>50</v>
       </c>
@@ -10006,11 +10383,11 @@
       </c>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
+      <c r="A80" s="12"/>
       <c r="B80" t="s">
         <v>50</v>
       </c>
-      <c r="C80" s="12">
+      <c r="C80" s="11">
         <v>71</v>
       </c>
       <c r="D80" s="2" t="str">
@@ -10115,7 +10492,7 @@
       </c>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="12"/>
       <c r="B81" t="s">
         <v>50</v>
       </c>
@@ -10224,7 +10601,7 @@
       </c>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B82" t="s">
@@ -10335,7 +10712,7 @@
       </c>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="12"/>
       <c r="B83" t="s">
         <v>50</v>
       </c>
@@ -10444,7 +10821,7 @@
       </c>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+      <c r="A84" s="12"/>
       <c r="B84" t="s">
         <v>50</v>
       </c>
@@ -10553,7 +10930,7 @@
       </c>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+      <c r="A85" s="12"/>
       <c r="B85" t="s">
         <v>50</v>
       </c>
@@ -10662,7 +11039,7 @@
       </c>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
+      <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>50</v>
       </c>
@@ -10771,7 +11148,7 @@
       </c>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+      <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>50</v>
       </c>
@@ -10880,7 +11257,7 @@
       </c>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+      <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>50</v>
       </c>
@@ -10989,7 +11366,7 @@
       </c>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
+      <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>50</v>
       </c>
@@ -11098,7 +11475,7 @@
       </c>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
+      <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>50</v>
       </c>
@@ -11207,11 +11584,11 @@
       </c>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
+      <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="12">
+      <c r="C91" s="11">
         <v>82</v>
       </c>
       <c r="D91" s="2" t="str">
@@ -11316,7 +11693,7 @@
       </c>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A92" s="11"/>
+      <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>50</v>
       </c>
@@ -11425,11 +11802,11 @@
       </c>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="11"/>
+      <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>50</v>
       </c>
-      <c r="C93" s="12">
+      <c r="C93" s="11">
         <v>84</v>
       </c>
       <c r="D93" s="2" t="str">
@@ -11534,7 +11911,7 @@
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="11"/>
+      <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>50</v>
       </c>
@@ -11643,7 +12020,7 @@
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B95" t="s">
@@ -11754,7 +12131,7 @@
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
+      <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>50</v>
       </c>
@@ -11863,7 +12240,7 @@
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A97" s="11"/>
+      <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>50</v>
       </c>
@@ -11972,7 +12349,7 @@
       </c>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
+      <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>50</v>
       </c>
@@ -12081,7 +12458,7 @@
       </c>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
+      <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>50</v>
       </c>
@@ -12190,7 +12567,7 @@
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A100" s="11"/>
+      <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>50</v>
       </c>
@@ -12299,7 +12676,7 @@
       </c>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
+      <c r="A101" s="12"/>
       <c r="B101" t="s">
         <v>50</v>
       </c>
@@ -12408,7 +12785,7 @@
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
+      <c r="A102" s="12"/>
       <c r="B102" t="s">
         <v>50</v>
       </c>
@@ -12517,7 +12894,7 @@
       </c>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
+      <c r="A103" s="12"/>
       <c r="B103" t="s">
         <v>50</v>
       </c>
@@ -12626,11 +13003,11 @@
       </c>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
+      <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>50</v>
       </c>
-      <c r="C104" s="12">
+      <c r="C104" s="11">
         <v>95</v>
       </c>
       <c r="D104" s="2" t="str">
@@ -12735,7 +13112,7 @@
       </c>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
+      <c r="A105" s="12"/>
       <c r="C105" s="2" t="s">
         <v>0</v>
       </c>
@@ -12836,7 +13213,7 @@
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
+      <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>50</v>
       </c>
@@ -12945,11 +13322,11 @@
       </c>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
+      <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>50</v>
       </c>
-      <c r="C107" s="12">
+      <c r="C107" s="11">
         <v>97</v>
       </c>
       <c r="D107" s="2" t="str">
@@ -13054,7 +13431,7 @@
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
+      <c r="A108" s="12"/>
       <c r="B108" t="s">
         <v>50</v>
       </c>
@@ -13163,7 +13540,7 @@
       </c>
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B109" t="s">
@@ -13274,11 +13651,11 @@
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
+      <c r="A110" s="12"/>
       <c r="B110" t="s">
         <v>50</v>
       </c>
-      <c r="C110" s="12">
+      <c r="C110" s="11">
         <v>100</v>
       </c>
       <c r="D110" s="2" t="str">
@@ -13383,7 +13760,7 @@
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
+      <c r="A111" s="12"/>
       <c r="B111" t="s">
         <v>50</v>
       </c>
@@ -13492,11 +13869,11 @@
       </c>
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
+      <c r="A112" s="12"/>
       <c r="B112" t="s">
         <v>50</v>
       </c>
-      <c r="C112" s="12">
+      <c r="C112" s="11">
         <v>102</v>
       </c>
       <c r="D112" s="2" t="str">
@@ -13601,7 +13978,7 @@
       </c>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A113" s="11"/>
+      <c r="A113" s="12"/>
       <c r="B113" t="s">
         <v>50</v>
       </c>
@@ -13710,7 +14087,7 @@
       </c>
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
+      <c r="A114" s="12"/>
       <c r="B114" t="s">
         <v>50</v>
       </c>
@@ -13819,7 +14196,7 @@
       </c>
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A115" s="11"/>
+      <c r="A115" s="12"/>
       <c r="B115" t="s">
         <v>50</v>
       </c>
@@ -13928,7 +14305,7 @@
       </c>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A116" s="11"/>
+      <c r="A116" s="12"/>
       <c r="B116" t="s">
         <v>50</v>
       </c>
@@ -14037,7 +14414,7 @@
       </c>
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A117" s="11"/>
+      <c r="A117" s="12"/>
       <c r="B117" t="s">
         <v>50</v>
       </c>
@@ -14146,7 +14523,7 @@
       </c>
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A118" s="11"/>
+      <c r="A118" s="12"/>
       <c r="B118" t="s">
         <v>50</v>
       </c>
@@ -14255,7 +14632,7 @@
       </c>
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A119" s="11"/>
+      <c r="A119" s="12"/>
       <c r="B119" t="s">
         <v>50</v>
       </c>
@@ -14364,11 +14741,11 @@
       </c>
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
+      <c r="A120" s="12"/>
       <c r="B120" t="s">
         <v>50</v>
       </c>
-      <c r="C120" s="12">
+      <c r="C120" s="11">
         <v>110</v>
       </c>
       <c r="D120" s="2" t="str">
@@ -14473,7 +14850,7 @@
       </c>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
+      <c r="A121" s="12"/>
       <c r="B121" t="s">
         <v>50</v>
       </c>
@@ -14582,11 +14959,11 @@
       </c>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A122" s="11"/>
+      <c r="A122" s="12"/>
       <c r="B122" t="s">
         <v>50</v>
       </c>
-      <c r="C122" s="12">
+      <c r="C122" s="11">
         <v>112</v>
       </c>
       <c r="D122" s="2" t="str">
@@ -14691,7 +15068,7 @@
       </c>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
+      <c r="A123" s="12"/>
       <c r="B123" t="s">
         <v>50</v>
       </c>
@@ -14800,7 +15177,7 @@
       </c>
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A124" s="11"/>
+      <c r="A124" s="12"/>
       <c r="B124" t="s">
         <v>50</v>
       </c>
@@ -14909,7 +15286,7 @@
       </c>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
+      <c r="A125" s="12"/>
       <c r="B125" t="s">
         <v>50</v>
       </c>
@@ -15018,7 +15395,7 @@
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A126" s="11"/>
+      <c r="A126" s="12"/>
       <c r="B126" t="s">
         <v>50</v>
       </c>
@@ -15127,7 +15504,7 @@
       </c>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
+      <c r="A127" s="12"/>
       <c r="B127" t="s">
         <v>50</v>
       </c>
@@ -15236,7 +15613,7 @@
       </c>
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="12"/>
       <c r="B128" t="s">
         <v>50</v>
       </c>
@@ -15345,11 +15722,11 @@
       </c>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
+      <c r="A129" s="12"/>
       <c r="B129" t="s">
         <v>50</v>
       </c>
-      <c r="C129" s="12">
+      <c r="C129" s="11">
         <v>119</v>
       </c>
       <c r="D129" s="2" t="str">
@@ -15454,7 +15831,7 @@
       </c>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
+      <c r="A130" s="12"/>
       <c r="B130" t="s">
         <v>50</v>
       </c>
@@ -15563,11 +15940,11 @@
       </c>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
+      <c r="A131" s="12"/>
       <c r="B131" t="s">
         <v>50</v>
       </c>
-      <c r="C131" s="12">
+      <c r="C131" s="11">
         <v>121</v>
       </c>
       <c r="D131" s="2" t="str">
@@ -15672,7 +16049,7 @@
       </c>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A132" s="11"/>
+      <c r="A132" s="12"/>
       <c r="B132" t="s">
         <v>50</v>
       </c>
@@ -15781,11 +16158,11 @@
       </c>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
+      <c r="A133" s="12"/>
       <c r="B133" t="s">
         <v>50</v>
       </c>
-      <c r="C133" s="12">
+      <c r="C133" s="11">
         <v>123</v>
       </c>
       <c r="D133" s="2" t="str">
@@ -15890,7 +16267,7 @@
       </c>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A134" s="11"/>
+      <c r="A134" s="12"/>
       <c r="B134" t="s">
         <v>50</v>
       </c>
@@ -15999,11 +16376,11 @@
       </c>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
+      <c r="A135" s="12"/>
       <c r="B135" t="s">
         <v>50</v>
       </c>
-      <c r="C135" s="12">
+      <c r="C135" s="11">
         <v>125</v>
       </c>
       <c r="D135" s="2" t="str">
@@ -16108,7 +16485,7 @@
       </c>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
+      <c r="A136" s="12"/>
       <c r="B136" t="s">
         <v>50</v>
       </c>
@@ -16217,7 +16594,7 @@
       </c>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A137" s="11" t="s">
+      <c r="A137" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B137" t="s">
@@ -16328,7 +16705,7 @@
       </c>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A138" s="11"/>
+      <c r="A138" s="12"/>
       <c r="C138" s="2" t="s">
         <v>0</v>
       </c>
@@ -16429,11 +16806,11 @@
       </c>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A139" s="11"/>
+      <c r="A139" s="12"/>
       <c r="B139" t="s">
         <v>50</v>
       </c>
-      <c r="C139" s="12">
+      <c r="C139" s="11">
         <v>128</v>
       </c>
       <c r="D139" s="2" t="str">
@@ -16538,7 +16915,7 @@
       </c>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
+      <c r="A140" s="12"/>
       <c r="B140" t="s">
         <v>50</v>
       </c>
@@ -16647,11 +17024,11 @@
       </c>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A141" s="11"/>
+      <c r="A141" s="12"/>
       <c r="B141" t="s">
         <v>50</v>
       </c>
-      <c r="C141" s="12">
+      <c r="C141" s="11">
         <v>130</v>
       </c>
       <c r="D141" s="2" t="str">
@@ -16756,7 +17133,7 @@
       </c>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A142" s="11"/>
+      <c r="A142" s="12"/>
       <c r="B142" t="s">
         <v>50</v>
       </c>
@@ -16865,7 +17242,7 @@
       </c>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B143" t="s">
@@ -16976,7 +17353,7 @@
       </c>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A144" s="11"/>
+      <c r="A144" s="12"/>
       <c r="B144" t="s">
         <v>50</v>
       </c>
@@ -17085,7 +17462,7 @@
       </c>
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A145" s="11"/>
+      <c r="A145" s="12"/>
       <c r="B145" t="s">
         <v>50</v>
       </c>
@@ -17194,7 +17571,7 @@
       </c>
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A146" s="11"/>
+      <c r="A146" s="12"/>
       <c r="B146" t="s">
         <v>50</v>
       </c>
@@ -17303,7 +17680,7 @@
       </c>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A147" s="11"/>
+      <c r="A147" s="12"/>
       <c r="B147" t="s">
         <v>50</v>
       </c>
@@ -17412,7 +17789,7 @@
       </c>
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A148" s="11"/>
+      <c r="A148" s="12"/>
       <c r="B148" t="s">
         <v>50</v>
       </c>
@@ -17521,7 +17898,7 @@
       </c>
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A149" s="11"/>
+      <c r="A149" s="12"/>
       <c r="B149" t="s">
         <v>50</v>
       </c>
@@ -17630,7 +18007,7 @@
       </c>
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A150" s="11" t="s">
+      <c r="A150" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B150" t="s">
@@ -17741,7 +18118,7 @@
       </c>
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
+      <c r="A151" s="12"/>
       <c r="B151" t="s">
         <v>50</v>
       </c>
@@ -17850,7 +18227,7 @@
       </c>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A152" s="11"/>
+      <c r="A152" s="12"/>
       <c r="B152" t="s">
         <v>50</v>
       </c>
@@ -17959,7 +18336,7 @@
       </c>
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A153" s="11"/>
+      <c r="A153" s="12"/>
       <c r="B153" t="s">
         <v>50</v>
       </c>
@@ -18068,7 +18445,7 @@
       </c>
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A154" s="11"/>
+      <c r="A154" s="12"/>
       <c r="B154" t="s">
         <v>50</v>
       </c>
@@ -18177,7 +18554,7 @@
       </c>
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A155" s="11"/>
+      <c r="A155" s="12"/>
       <c r="B155" t="s">
         <v>50</v>
       </c>
@@ -18286,7 +18663,7 @@
       </c>
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A156" s="11" t="s">
+      <c r="A156" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B156" t="s">
@@ -18397,11 +18774,11 @@
       </c>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A157" s="11"/>
+      <c r="A157" s="12"/>
       <c r="B157" t="s">
         <v>50</v>
       </c>
-      <c r="C157" s="12">
+      <c r="C157" s="11">
         <v>146</v>
       </c>
       <c r="D157" s="2" t="str">
@@ -18506,7 +18883,7 @@
       </c>
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A158" s="11"/>
+      <c r="A158" s="12"/>
       <c r="B158" t="s">
         <v>50</v>
       </c>
@@ -18615,7 +18992,7 @@
       </c>
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B159" t="s">
@@ -18726,7 +19103,7 @@
       </c>
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A160" s="11"/>
+      <c r="A160" s="12"/>
       <c r="B160" t="s">
         <v>50</v>
       </c>
@@ -18835,11 +19212,11 @@
       </c>
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A161" s="11"/>
+      <c r="A161" s="12"/>
       <c r="B161" t="s">
         <v>50</v>
       </c>
-      <c r="C161" s="12">
+      <c r="C161" s="11">
         <v>150</v>
       </c>
       <c r="D161" s="2" t="str">
@@ -18944,7 +19321,7 @@
       </c>
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A162" s="11"/>
+      <c r="A162" s="12"/>
       <c r="B162" t="s">
         <v>50</v>
       </c>
@@ -19053,7 +19430,7 @@
       </c>
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A163" s="11" t="s">
+      <c r="A163" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B163" t="s">
@@ -19164,11 +19541,11 @@
       </c>
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A164" s="11"/>
+      <c r="A164" s="12"/>
       <c r="B164" t="s">
         <v>50</v>
       </c>
-      <c r="C164" s="12">
+      <c r="C164" s="11">
         <v>153</v>
       </c>
       <c r="D164" s="2" t="str">
@@ -19273,7 +19650,7 @@
       </c>
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A165" s="11"/>
+      <c r="A165" s="12"/>
       <c r="B165" t="s">
         <v>50</v>
       </c>
@@ -19382,7 +19759,7 @@
       </c>
     </row>
     <row r="166" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A166" s="11" t="s">
+      <c r="A166" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B166" t="s">
@@ -19493,7 +19870,7 @@
       </c>
     </row>
     <row r="167" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A167" s="11"/>
+      <c r="A167" s="12"/>
       <c r="B167" t="s">
         <v>50</v>
       </c>
@@ -19602,11 +19979,11 @@
       </c>
     </row>
     <row r="168" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A168" s="11"/>
+      <c r="A168" s="12"/>
       <c r="B168" t="s">
         <v>50</v>
       </c>
-      <c r="C168" s="12">
+      <c r="C168" s="11">
         <v>157</v>
       </c>
       <c r="D168" s="2" t="str">
@@ -19711,7 +20088,7 @@
       </c>
     </row>
     <row r="169" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A169" s="11"/>
+      <c r="A169" s="12"/>
       <c r="B169" t="s">
         <v>50</v>
       </c>
@@ -20031,6 +20408,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A163:A165"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="A109:A136"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A143:A149"/>
+    <mergeCell ref="A150:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A159:A162"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="A69:A81"/>
+    <mergeCell ref="A82:A94"/>
+    <mergeCell ref="A95:A108"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A52:A56"/>
     <mergeCell ref="A20:A26"/>
     <mergeCell ref="A37:A44"/>
     <mergeCell ref="A50:A51"/>
@@ -20039,20 +20430,6 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="A69:A81"/>
-    <mergeCell ref="A82:A94"/>
-    <mergeCell ref="A95:A108"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A163:A165"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="A109:A136"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A143:A149"/>
-    <mergeCell ref="A150:A155"/>
-    <mergeCell ref="A156:A158"/>
-    <mergeCell ref="A159:A162"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
@@ -20063,13 +20440,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H130" workbookViewId="0">
-      <selection activeCell="AB142" sqref="AB142"/>
+    <sheetView tabSelected="1" topLeftCell="U130" workbookViewId="0">
+      <selection activeCell="AA135" sqref="AA135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="21" max="22" width="11.140625" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="28" max="29" width="9.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="11.85546875" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -20303,8 +20701,12 @@
       <c r="T6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
+      <c r="U6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="W6" s="5" t="s">
         <v>3</v>
       </c>
@@ -20664,7 +21066,7 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -20775,7 +21177,7 @@
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -20884,7 +21286,7 @@
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -20993,7 +21395,7 @@
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>50</v>
       </c>
@@ -21102,7 +21504,7 @@
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -21211,7 +21613,7 @@
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="12">
         <v>5</v>
       </c>
       <c r="B15" t="s">
@@ -21322,7 +21724,7 @@
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -21431,7 +21833,7 @@
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" t="s">
         <v>50</v>
       </c>
@@ -21540,7 +21942,7 @@
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -21649,7 +22051,7 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -21758,7 +22160,7 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
@@ -21869,7 +22271,7 @@
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -21978,7 +22380,7 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -22087,7 +22489,7 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -22196,7 +22598,7 @@
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -22305,7 +22707,7 @@
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -22414,7 +22816,7 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -22523,7 +22925,7 @@
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="12">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -22634,7 +23036,7 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -22743,7 +23145,7 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>50</v>
       </c>
@@ -22852,7 +23254,7 @@
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" t="s">
         <v>50</v>
       </c>
@@ -22961,7 +23363,7 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>50</v>
       </c>
@@ -23070,7 +23472,7 @@
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="12">
         <v>5</v>
       </c>
       <c r="B32" t="s">
@@ -23181,7 +23583,7 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -23290,7 +23692,7 @@
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -23399,7 +23801,7 @@
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -23508,7 +23910,7 @@
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -23617,7 +24019,7 @@
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
@@ -23728,7 +24130,7 @@
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -23837,7 +24239,7 @@
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -23946,7 +24348,7 @@
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="12"/>
       <c r="B40" t="s">
         <v>50</v>
       </c>
@@ -24055,7 +24457,7 @@
       </c>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="12"/>
       <c r="B41" t="s">
         <v>50</v>
       </c>
@@ -24164,7 +24566,7 @@
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="12"/>
       <c r="B42" t="s">
         <v>50</v>
       </c>
@@ -24273,7 +24675,7 @@
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="12"/>
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -24382,7 +24784,7 @@
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="A44" s="12">
         <v>5</v>
       </c>
       <c r="B44" t="s">
@@ -24493,7 +24895,7 @@
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>50</v>
       </c>
@@ -24602,7 +25004,7 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -24711,7 +25113,7 @@
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>50</v>
       </c>
@@ -24820,7 +25222,7 @@
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+      <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>50</v>
       </c>
@@ -24929,7 +25331,7 @@
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B49" t="s">
@@ -25040,7 +25442,7 @@
       </c>
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+      <c r="A50" s="12"/>
       <c r="B50" t="s">
         <v>50</v>
       </c>
@@ -25149,7 +25551,7 @@
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B51" t="s">
@@ -25260,7 +25662,7 @@
       </c>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+      <c r="A52" s="12"/>
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -25369,7 +25771,7 @@
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
+      <c r="A53" s="12"/>
       <c r="B53" t="s">
         <v>50</v>
       </c>
@@ -25478,7 +25880,7 @@
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
+      <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -25587,7 +25989,7 @@
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+      <c r="A55" s="12"/>
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -25696,7 +26098,7 @@
       </c>
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B56" t="s">
@@ -25807,7 +26209,7 @@
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
+      <c r="A57" s="12"/>
       <c r="B57" t="s">
         <v>50</v>
       </c>
@@ -25916,7 +26318,7 @@
       </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
+      <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -26025,7 +26427,7 @@
       </c>
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
+      <c r="A59" s="12"/>
       <c r="B59" t="s">
         <v>50</v>
       </c>
@@ -26134,7 +26536,7 @@
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+      <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -26243,7 +26645,7 @@
       </c>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -26354,7 +26756,7 @@
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
+      <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>50</v>
       </c>
@@ -26463,7 +26865,7 @@
       </c>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
+      <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>50</v>
       </c>
@@ -26572,7 +26974,7 @@
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
+      <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>50</v>
       </c>
@@ -26681,7 +27083,7 @@
       </c>
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
+      <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>50</v>
       </c>
@@ -26790,7 +27192,7 @@
       </c>
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
+      <c r="A66" s="12"/>
       <c r="B66" t="s">
         <v>50</v>
       </c>
@@ -26899,7 +27301,7 @@
       </c>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+      <c r="A67" s="12"/>
       <c r="B67" t="s">
         <v>50</v>
       </c>
@@ -27008,7 +27410,7 @@
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B68" t="s">
@@ -27119,7 +27521,7 @@
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
+      <c r="A69" s="12"/>
       <c r="B69" t="s">
         <v>50</v>
       </c>
@@ -27228,7 +27630,7 @@
       </c>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
+      <c r="A70" s="12"/>
       <c r="B70" t="s">
         <v>50</v>
       </c>
@@ -27337,7 +27739,7 @@
       </c>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
+      <c r="A71" s="12"/>
       <c r="B71" t="s">
         <v>50</v>
       </c>
@@ -27446,7 +27848,7 @@
       </c>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+      <c r="A72" s="12"/>
       <c r="B72" t="s">
         <v>50</v>
       </c>
@@ -27555,7 +27957,7 @@
       </c>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
+      <c r="A73" s="12"/>
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -27664,7 +28066,7 @@
       </c>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
+      <c r="A74" s="12"/>
       <c r="B74" t="s">
         <v>50</v>
       </c>
@@ -27773,7 +28175,7 @@
       </c>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
+      <c r="A75" s="12"/>
       <c r="B75" t="s">
         <v>50</v>
       </c>
@@ -27882,7 +28284,7 @@
       </c>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+      <c r="A76" s="12"/>
       <c r="B76" t="s">
         <v>50</v>
       </c>
@@ -27991,7 +28393,7 @@
       </c>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+      <c r="A77" s="12"/>
       <c r="B77" t="s">
         <v>50</v>
       </c>
@@ -28100,7 +28502,7 @@
       </c>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+      <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>50</v>
       </c>
@@ -28209,7 +28611,7 @@
       </c>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
+      <c r="A79" s="12"/>
       <c r="B79" t="s">
         <v>50</v>
       </c>
@@ -28318,7 +28720,7 @@
       </c>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B80" t="s">
@@ -28429,7 +28831,7 @@
       </c>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="12"/>
       <c r="B81" t="s">
         <v>50</v>
       </c>
@@ -28538,7 +28940,7 @@
       </c>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="12"/>
       <c r="B82" t="s">
         <v>50</v>
       </c>
@@ -28647,7 +29049,7 @@
       </c>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="12"/>
       <c r="B83" t="s">
         <v>50</v>
       </c>
@@ -28756,7 +29158,7 @@
       </c>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+      <c r="A84" s="12"/>
       <c r="B84" t="s">
         <v>50</v>
       </c>
@@ -28865,7 +29267,7 @@
       </c>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+      <c r="A85" s="12"/>
       <c r="B85" t="s">
         <v>50</v>
       </c>
@@ -28974,7 +29376,7 @@
       </c>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
+      <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>50</v>
       </c>
@@ -29083,7 +29485,7 @@
       </c>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+      <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>50</v>
       </c>
@@ -29192,7 +29594,7 @@
       </c>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+      <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>50</v>
       </c>
@@ -29301,7 +29703,7 @@
       </c>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
+      <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>50</v>
       </c>
@@ -29410,7 +29812,7 @@
       </c>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
+      <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>50</v>
       </c>
@@ -29519,7 +29921,7 @@
       </c>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
+      <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>50</v>
       </c>
@@ -29628,7 +30030,7 @@
       </c>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A92" s="11"/>
+      <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>50</v>
       </c>
@@ -29737,7 +30139,7 @@
       </c>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B93" t="s">
@@ -29848,7 +30250,7 @@
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="11"/>
+      <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>50</v>
       </c>
@@ -29957,7 +30359,7 @@
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
+      <c r="A95" s="12"/>
       <c r="B95" t="s">
         <v>50</v>
       </c>
@@ -30066,7 +30468,7 @@
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
+      <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>50</v>
       </c>
@@ -30175,7 +30577,7 @@
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A97" s="11"/>
+      <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>50</v>
       </c>
@@ -30284,7 +30686,7 @@
       </c>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
+      <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>50</v>
       </c>
@@ -30393,7 +30795,7 @@
       </c>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
+      <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>50</v>
       </c>
@@ -30502,7 +30904,7 @@
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A100" s="11"/>
+      <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>50</v>
       </c>
@@ -30611,7 +31013,7 @@
       </c>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
+      <c r="A101" s="12"/>
       <c r="B101" t="s">
         <v>50</v>
       </c>
@@ -30720,7 +31122,7 @@
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
+      <c r="A102" s="12"/>
       <c r="B102" t="s">
         <v>50</v>
       </c>
@@ -30829,7 +31231,7 @@
       </c>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
+      <c r="A103" s="12"/>
       <c r="B103" t="s">
         <v>50</v>
       </c>
@@ -30938,7 +31340,7 @@
       </c>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
+      <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>50</v>
       </c>
@@ -31047,7 +31449,7 @@
       </c>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
+      <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>50</v>
       </c>
@@ -31156,7 +31558,7 @@
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
+      <c r="A106" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B106" t="s">
@@ -31267,7 +31669,7 @@
       </c>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
+      <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>50</v>
       </c>
@@ -31376,7 +31778,7 @@
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
+      <c r="A108" s="12"/>
       <c r="B108" t="s">
         <v>50</v>
       </c>
@@ -31485,7 +31887,7 @@
       </c>
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A109" s="11"/>
+      <c r="A109" s="12"/>
       <c r="B109" t="s">
         <v>50</v>
       </c>
@@ -31594,7 +31996,7 @@
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
+      <c r="A110" s="12"/>
       <c r="B110" t="s">
         <v>50</v>
       </c>
@@ -31703,7 +32105,7 @@
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
+      <c r="A111" s="12"/>
       <c r="B111" t="s">
         <v>50</v>
       </c>
@@ -31812,7 +32214,7 @@
       </c>
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
+      <c r="A112" s="12"/>
       <c r="B112" t="s">
         <v>50</v>
       </c>
@@ -31921,7 +32323,7 @@
       </c>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A113" s="11"/>
+      <c r="A113" s="12"/>
       <c r="B113" t="s">
         <v>50</v>
       </c>
@@ -32030,7 +32432,7 @@
       </c>
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
+      <c r="A114" s="12"/>
       <c r="B114" t="s">
         <v>50</v>
       </c>
@@ -32139,7 +32541,7 @@
       </c>
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A115" s="11"/>
+      <c r="A115" s="12"/>
       <c r="B115" t="s">
         <v>50</v>
       </c>
@@ -32248,7 +32650,7 @@
       </c>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A116" s="11"/>
+      <c r="A116" s="12"/>
       <c r="B116" t="s">
         <v>50</v>
       </c>
@@ -32357,7 +32759,7 @@
       </c>
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A117" s="11"/>
+      <c r="A117" s="12"/>
       <c r="B117" t="s">
         <v>50</v>
       </c>
@@ -32466,7 +32868,7 @@
       </c>
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A118" s="11"/>
+      <c r="A118" s="12"/>
       <c r="B118" t="s">
         <v>50</v>
       </c>
@@ -32575,7 +32977,7 @@
       </c>
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A119" s="11"/>
+      <c r="A119" s="12"/>
       <c r="B119" t="s">
         <v>50</v>
       </c>
@@ -32684,7 +33086,7 @@
       </c>
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
+      <c r="A120" s="12"/>
       <c r="B120" t="s">
         <v>50</v>
       </c>
@@ -32793,7 +33195,7 @@
       </c>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
+      <c r="A121" s="12"/>
       <c r="B121" t="s">
         <v>50</v>
       </c>
@@ -32902,7 +33304,7 @@
       </c>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A122" s="11"/>
+      <c r="A122" s="12"/>
       <c r="B122" t="s">
         <v>50</v>
       </c>
@@ -33011,7 +33413,7 @@
       </c>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
+      <c r="A123" s="12"/>
       <c r="B123" t="s">
         <v>50</v>
       </c>
@@ -33120,7 +33522,7 @@
       </c>
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A124" s="11"/>
+      <c r="A124" s="12"/>
       <c r="B124" t="s">
         <v>50</v>
       </c>
@@ -33229,7 +33631,7 @@
       </c>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
+      <c r="A125" s="12"/>
       <c r="B125" t="s">
         <v>50</v>
       </c>
@@ -33338,7 +33740,7 @@
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A126" s="11"/>
+      <c r="A126" s="12"/>
       <c r="B126" t="s">
         <v>50</v>
       </c>
@@ -33447,7 +33849,7 @@
       </c>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
+      <c r="A127" s="12"/>
       <c r="B127" t="s">
         <v>50</v>
       </c>
@@ -33556,7 +33958,7 @@
       </c>
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="12"/>
       <c r="B128" t="s">
         <v>50</v>
       </c>
@@ -33665,7 +34067,7 @@
       </c>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
+      <c r="A129" s="12"/>
       <c r="B129" t="s">
         <v>50</v>
       </c>
@@ -33774,7 +34176,7 @@
       </c>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
+      <c r="A130" s="12"/>
       <c r="B130" t="s">
         <v>50</v>
       </c>
@@ -33883,7 +34285,7 @@
       </c>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
+      <c r="A131" s="12"/>
       <c r="B131" t="s">
         <v>50</v>
       </c>
@@ -33992,7 +34394,7 @@
       </c>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A132" s="11"/>
+      <c r="A132" s="12"/>
       <c r="B132" t="s">
         <v>50</v>
       </c>
@@ -34101,7 +34503,7 @@
       </c>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
+      <c r="A133" s="12"/>
       <c r="B133" t="s">
         <v>50</v>
       </c>
@@ -34210,7 +34612,7 @@
       </c>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A134" s="11" t="s">
+      <c r="A134" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B134" t="s">
@@ -34233,10 +34635,10 @@
         <v>0</v>
       </c>
       <c r="H134" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I134" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J134" s="3">
         <v>0</v>
@@ -34290,13 +34692,13 @@
         <v>0</v>
       </c>
       <c r="AA134" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB134" s="6">
         <v>0</v>
       </c>
       <c r="AC134" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD134" s="5">
         <v>0</v>
@@ -34317,11 +34719,11 @@
         <v>0</v>
       </c>
       <c r="AJ134" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
+      <c r="A135" s="12"/>
       <c r="B135" t="s">
         <v>50</v>
       </c>
@@ -34336,16 +34738,16 @@
         <v>0</v>
       </c>
       <c r="F135" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G135" s="4">
         <v>0</v>
       </c>
       <c r="H135" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I135" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135" s="3">
         <v>0</v>
@@ -34399,13 +34801,13 @@
         <v>0</v>
       </c>
       <c r="AA135" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB135" s="6">
         <v>0</v>
       </c>
       <c r="AC135" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD135" s="5">
         <v>0</v>
@@ -34426,11 +34828,11 @@
         <v>0</v>
       </c>
       <c r="AJ135" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
+      <c r="A136" s="12"/>
       <c r="B136" t="s">
         <v>50</v>
       </c>
@@ -34445,19 +34847,19 @@
         <v>0</v>
       </c>
       <c r="F136" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G136" s="4">
         <v>0</v>
       </c>
       <c r="H136" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I136" s="3">
         <v>0</v>
       </c>
       <c r="J136" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K136" s="3">
         <v>0</v>
@@ -34508,13 +34910,13 @@
         <v>0</v>
       </c>
       <c r="AA136" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB136" s="6">
         <v>0</v>
       </c>
       <c r="AC136" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD136" s="5">
         <v>0</v>
@@ -34535,11 +34937,11 @@
         <v>0</v>
       </c>
       <c r="AJ136" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A137" s="11"/>
+      <c r="A137" s="12"/>
       <c r="B137" t="s">
         <v>50</v>
       </c>
@@ -34554,19 +34956,19 @@
         <v>0</v>
       </c>
       <c r="F137" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" s="4">
         <v>0</v>
       </c>
       <c r="H137" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" s="3">
         <v>0</v>
       </c>
       <c r="J137" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K137" s="3">
         <v>0</v>
@@ -34617,13 +35019,13 @@
         <v>0</v>
       </c>
       <c r="AA137" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB137" s="6">
         <v>0</v>
       </c>
       <c r="AC137" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD137" s="5">
         <v>0</v>
@@ -34644,11 +35046,11 @@
         <v>0</v>
       </c>
       <c r="AJ137" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A138" s="11"/>
+      <c r="A138" s="12"/>
       <c r="B138" t="s">
         <v>50</v>
       </c>
@@ -34663,7 +35065,7 @@
         <v>0</v>
       </c>
       <c r="F138" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G138" s="4">
         <v>0</v>
@@ -34757,7 +35159,7 @@
       </c>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A139" s="11" t="s">
+      <c r="A139" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B139" t="s">
@@ -34868,7 +35270,7 @@
       </c>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
+      <c r="A140" s="12"/>
       <c r="B140" t="s">
         <v>50</v>
       </c>
@@ -34977,7 +35379,7 @@
       </c>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A141" s="11"/>
+      <c r="A141" s="12"/>
       <c r="B141" t="s">
         <v>50</v>
       </c>
@@ -35086,7 +35488,7 @@
       </c>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A142" s="11"/>
+      <c r="A142" s="12"/>
       <c r="B142" t="s">
         <v>50</v>
       </c>
@@ -35195,7 +35597,7 @@
       </c>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A143" s="11"/>
+      <c r="A143" s="12"/>
       <c r="B143" t="s">
         <v>50</v>
       </c>
@@ -35304,7 +35706,7 @@
       </c>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A144" s="11"/>
+      <c r="A144" s="12"/>
       <c r="B144" t="s">
         <v>50</v>
       </c>
@@ -35413,7 +35815,7 @@
       </c>
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A145" s="11"/>
+      <c r="A145" s="12"/>
       <c r="B145" t="s">
         <v>50</v>
       </c>
@@ -35522,7 +35924,7 @@
       </c>
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A146" s="11" t="s">
+      <c r="A146" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B146" t="s">
@@ -35633,7 +36035,7 @@
       </c>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A147" s="11"/>
+      <c r="A147" s="12"/>
       <c r="B147" t="s">
         <v>50</v>
       </c>
@@ -35742,7 +36144,7 @@
       </c>
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A148" s="11"/>
+      <c r="A148" s="12"/>
       <c r="B148" t="s">
         <v>50</v>
       </c>
@@ -35851,7 +36253,7 @@
       </c>
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A149" s="11"/>
+      <c r="A149" s="12"/>
       <c r="B149" t="s">
         <v>50</v>
       </c>
@@ -35960,7 +36362,7 @@
       </c>
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A150" s="11"/>
+      <c r="A150" s="12"/>
       <c r="B150" t="s">
         <v>50</v>
       </c>
@@ -36069,7 +36471,7 @@
       </c>
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
+      <c r="A151" s="12"/>
       <c r="B151" t="s">
         <v>50</v>
       </c>
@@ -36178,7 +36580,7 @@
       </c>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A152" s="11" t="s">
+      <c r="A152" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B152" t="s">
@@ -36289,7 +36691,7 @@
       </c>
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A153" s="11"/>
+      <c r="A153" s="12"/>
       <c r="B153" t="s">
         <v>50</v>
       </c>
@@ -36398,7 +36800,7 @@
       </c>
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A154" s="11"/>
+      <c r="A154" s="12"/>
       <c r="B154" t="s">
         <v>50</v>
       </c>
@@ -36507,7 +36909,7 @@
       </c>
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A155" s="11" t="s">
+      <c r="A155" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B155" t="s">
@@ -36618,7 +37020,7 @@
       </c>
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A156" s="11"/>
+      <c r="A156" s="12"/>
       <c r="B156" t="s">
         <v>50</v>
       </c>
@@ -36727,7 +37129,7 @@
       </c>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A157" s="11"/>
+      <c r="A157" s="12"/>
       <c r="B157" t="s">
         <v>50</v>
       </c>
@@ -36836,7 +37238,7 @@
       </c>
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A158" s="11"/>
+      <c r="A158" s="12"/>
       <c r="B158" t="s">
         <v>50</v>
       </c>
@@ -36945,7 +37347,7 @@
       </c>
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B159" t="s">
@@ -37056,7 +37458,7 @@
       </c>
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A160" s="11"/>
+      <c r="A160" s="12"/>
       <c r="B160" t="s">
         <v>50</v>
       </c>
@@ -37165,7 +37567,7 @@
       </c>
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A161" s="11"/>
+      <c r="A161" s="12"/>
       <c r="B161" t="s">
         <v>50</v>
       </c>
@@ -37274,7 +37676,7 @@
       </c>
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A162" s="11" t="s">
+      <c r="A162" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B162" t="s">
@@ -37385,7 +37787,7 @@
       </c>
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A163" s="11"/>
+      <c r="A163" s="12"/>
       <c r="B163" t="s">
         <v>50</v>
       </c>
@@ -37494,7 +37896,7 @@
       </c>
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A164" s="11"/>
+      <c r="A164" s="12"/>
       <c r="B164" t="s">
         <v>50</v>
       </c>
@@ -37603,7 +38005,7 @@
       </c>
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A165" s="11"/>
+      <c r="A165" s="12"/>
       <c r="B165" t="s">
         <v>50</v>
       </c>
@@ -37923,6 +38325,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A68:A79"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A61:A67"/>
     <mergeCell ref="A152:A154"/>
     <mergeCell ref="A155:A158"/>
     <mergeCell ref="A159:A161"/>
@@ -37933,20 +38347,11 @@
     <mergeCell ref="A134:A138"/>
     <mergeCell ref="A139:A145"/>
     <mergeCell ref="A146:A151"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A79"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A43"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Todos os bugs principais consertados. Versão beta 1.0.
</commit_message>
<xml_diff>
--- a/Files/instruction_mapping.xlsx
+++ b/Files/instruction_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\M3PlusMicrocontroller\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M3PlusMicrocontrollerSimulator\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1017,10 +1017,10 @@
     <t>HD, 1, 4</t>
   </si>
   <si>
-    <t>Colunas1</t>
+    <t>---</t>
   </si>
   <si>
-    <t>Colunas2</t>
+    <t>----</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1176,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1392,6 +1392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1553,7 +1559,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1588,6 +1594,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1635,24 +1653,6 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1959,6 +1959,24 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1973,46 +1991,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B6:AJ166" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B6:AJ166" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B6:AJ166"/>
   <tableColumns count="35">
     <tableColumn id="1" name="Operação/Fluxo"/>
-    <tableColumn id="2" name="Dec" dataDxfId="35"/>
-    <tableColumn id="3" name="Hex" dataDxfId="34">
+    <tableColumn id="2" name="Dec" dataDxfId="33"/>
+    <tableColumn id="3" name="Hex" dataDxfId="32">
       <calculatedColumnFormula>DEC2HEX(C7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="SPIncDec" dataDxfId="33"/>
-    <tableColumn id="5" name="SP clock" dataDxfId="32"/>
-    <tableColumn id="6" name="DIRClock" dataDxfId="31"/>
-    <tableColumn id="7" name="SelDataPC" dataDxfId="30"/>
-    <tableColumn id="8" name="Clock PCL" dataDxfId="29"/>
-    <tableColumn id="9" name="Clock PCH" dataDxfId="28"/>
-    <tableColumn id="10" name="PCL Bus" dataDxfId="27"/>
-    <tableColumn id="11" name="PCH Bus" dataDxfId="26"/>
-    <tableColumn id="12" name="ROM cs" dataDxfId="25"/>
-    <tableColumn id="13" name="ROM rd" dataDxfId="24"/>
-    <tableColumn id="14" name="HD clock" dataDxfId="23"/>
-    <tableColumn id="15" name="SelRI" dataDxfId="22"/>
-    <tableColumn id="16" name="RIClock" dataDxfId="21"/>
-    <tableColumn id="17" name="CresZ" dataDxfId="20"/>
-    <tableColumn id="18" name="CresC" dataDxfId="19"/>
-    <tableColumn id="19" name="Cres" dataDxfId="18"/>
-    <tableColumn id="20" name="Colunas1" dataDxfId="17"/>
-    <tableColumn id="21" name="Colunas2" dataDxfId="16"/>
-    <tableColumn id="22" name="HD res" dataDxfId="15"/>
-    <tableColumn id="23" name="HD" dataDxfId="14"/>
-    <tableColumn id="24" name="Out clock" dataDxfId="13"/>
-    <tableColumn id="25" name="IN Bus" dataDxfId="12"/>
-    <tableColumn id="26" name="RAM cs" dataDxfId="11"/>
-    <tableColumn id="27" name="Ram wr" dataDxfId="10"/>
-    <tableColumn id="28" name="RAM rd" dataDxfId="9"/>
-    <tableColumn id="29" name="Reg Clock" dataDxfId="8"/>
-    <tableColumn id="30" name="Reg Bus" dataDxfId="7"/>
-    <tableColumn id="31" name="AC Clock" dataDxfId="6"/>
-    <tableColumn id="32" name="AC Bus" dataDxfId="5"/>
-    <tableColumn id="33" name="BUF Clock" dataDxfId="4"/>
-    <tableColumn id="34" name="ULA Bus" dataDxfId="3"/>
-    <tableColumn id="35" name="Sel SP" dataDxfId="2"/>
+    <tableColumn id="4" name="SPIncDec" dataDxfId="31"/>
+    <tableColumn id="5" name="SP clock" dataDxfId="30"/>
+    <tableColumn id="6" name="DIRClock" dataDxfId="29"/>
+    <tableColumn id="7" name="SelDataPC" dataDxfId="28"/>
+    <tableColumn id="8" name="Clock PCL" dataDxfId="27"/>
+    <tableColumn id="9" name="Clock PCH" dataDxfId="26"/>
+    <tableColumn id="10" name="PCL Bus" dataDxfId="25"/>
+    <tableColumn id="11" name="PCH Bus" dataDxfId="24"/>
+    <tableColumn id="12" name="ROM cs" dataDxfId="23"/>
+    <tableColumn id="13" name="ROM rd" dataDxfId="22"/>
+    <tableColumn id="14" name="HD clock" dataDxfId="21"/>
+    <tableColumn id="15" name="SelRI" dataDxfId="20"/>
+    <tableColumn id="16" name="RIClock" dataDxfId="19"/>
+    <tableColumn id="17" name="CresZ" dataDxfId="18"/>
+    <tableColumn id="18" name="CresC" dataDxfId="17"/>
+    <tableColumn id="19" name="Cres" dataDxfId="16"/>
+    <tableColumn id="20" name="---" dataDxfId="15"/>
+    <tableColumn id="21" name="----" dataDxfId="14"/>
+    <tableColumn id="22" name="HD res" dataDxfId="13"/>
+    <tableColumn id="23" name="HD" dataDxfId="12"/>
+    <tableColumn id="24" name="Out clock" dataDxfId="11"/>
+    <tableColumn id="25" name="IN Bus" dataDxfId="10"/>
+    <tableColumn id="26" name="RAM cs" dataDxfId="9"/>
+    <tableColumn id="27" name="Ram wr" dataDxfId="8"/>
+    <tableColumn id="28" name="RAM rd" dataDxfId="7"/>
+    <tableColumn id="29" name="Reg Clock" dataDxfId="6"/>
+    <tableColumn id="30" name="Reg Bus" dataDxfId="5"/>
+    <tableColumn id="31" name="AC Clock" dataDxfId="4"/>
+    <tableColumn id="32" name="AC Bus" dataDxfId="3"/>
+    <tableColumn id="33" name="BUF Clock" dataDxfId="2"/>
+    <tableColumn id="34" name="ULA Bus" dataDxfId="1"/>
+    <tableColumn id="35" name="Sel SP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20408,6 +20426,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="A69:A81"/>
+    <mergeCell ref="A82:A94"/>
+    <mergeCell ref="A95:A108"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A52:A56"/>
     <mergeCell ref="A163:A165"/>
     <mergeCell ref="A166:A169"/>
     <mergeCell ref="A109:A136"/>
@@ -20416,20 +20448,6 @@
     <mergeCell ref="A150:A155"/>
     <mergeCell ref="A156:A158"/>
     <mergeCell ref="A159:A162"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="A69:A81"/>
-    <mergeCell ref="A82:A94"/>
-    <mergeCell ref="A95:A108"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
@@ -20440,8 +20458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U130" workbookViewId="0">
-      <selection activeCell="AA135" sqref="AA135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20647,106 +20665,106 @@
       <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="X6" s="5" t="s">
+      <c r="X6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Y6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="Z6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AA6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AB6" s="6" t="s">
+      <c r="AB6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AC6" s="5" t="s">
+      <c r="AC6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="AD6" s="5" t="s">
+      <c r="AD6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AE6" s="5" t="s">
+      <c r="AE6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="5" t="s">
+      <c r="AF6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AG6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AH6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AI6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22180,7 +22198,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
@@ -22289,7 +22307,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4">
         <v>0</v>
@@ -26882,8 +26900,8 @@
       <c r="F63" s="4">
         <v>0</v>
       </c>
-      <c r="G63" s="4">
-        <v>0</v>
+      <c r="G63" s="16">
+        <v>1</v>
       </c>
       <c r="H63" s="4">
         <v>0</v>
@@ -26992,7 +27010,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="4">
         <v>0</v>
@@ -29615,10 +29633,10 @@
         <v>0</v>
       </c>
       <c r="H88" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J88" s="3">
         <v>0</v>
@@ -29648,7 +29666,7 @@
         <v>0</v>
       </c>
       <c r="S88" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T88" s="3">
         <v>0</v>
@@ -29672,13 +29690,13 @@
         <v>0</v>
       </c>
       <c r="AA88" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB88" s="6">
         <v>0</v>
       </c>
       <c r="AC88" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD88" s="5">
         <v>0</v>
@@ -29699,7 +29717,7 @@
         <v>0</v>
       </c>
       <c r="AJ88" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
@@ -29718,16 +29736,16 @@
         <v>0</v>
       </c>
       <c r="F89" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" s="4">
         <v>0</v>
       </c>
       <c r="H89" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89" s="3">
         <v>0</v>
@@ -29781,13 +29799,13 @@
         <v>0</v>
       </c>
       <c r="AA89" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB89" s="6">
         <v>0</v>
       </c>
       <c r="AC89" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD89" s="5">
         <v>0</v>
@@ -29808,7 +29826,7 @@
         <v>0</v>
       </c>
       <c r="AJ89" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
@@ -29827,19 +29845,19 @@
         <v>0</v>
       </c>
       <c r="F90" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="4">
         <v>0</v>
       </c>
       <c r="H90" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" s="3">
         <v>0</v>
       </c>
       <c r="J90" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K90" s="3">
         <v>0</v>
@@ -29890,13 +29908,13 @@
         <v>0</v>
       </c>
       <c r="AA90" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB90" s="6">
         <v>0</v>
       </c>
       <c r="AC90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD90" s="5">
         <v>0</v>
@@ -29917,7 +29935,7 @@
         <v>0</v>
       </c>
       <c r="AJ90" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
@@ -29936,19 +29954,19 @@
         <v>0</v>
       </c>
       <c r="F91" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" s="4">
         <v>0</v>
       </c>
       <c r="H91" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" s="3">
         <v>0</v>
       </c>
       <c r="J91" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K91" s="3">
         <v>0</v>
@@ -29999,13 +30017,13 @@
         <v>0</v>
       </c>
       <c r="AA91" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB91" s="6">
         <v>0</v>
       </c>
       <c r="AC91" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD91" s="5">
         <v>0</v>
@@ -30026,7 +30044,7 @@
         <v>0</v>
       </c>
       <c r="AJ91" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
@@ -30045,7 +30063,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="4">
         <v>0</v>
@@ -30084,7 +30102,7 @@
         <v>0</v>
       </c>
       <c r="S92" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T92" s="3">
         <v>1</v>
@@ -31034,7 +31052,7 @@
         <v>0</v>
       </c>
       <c r="H101" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" s="3">
         <v>0</v>
@@ -31064,7 +31082,7 @@
         <v>0</v>
       </c>
       <c r="R101" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S101" s="3">
         <v>0</v>
@@ -31091,13 +31109,13 @@
         <v>0</v>
       </c>
       <c r="AA101" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB101" s="6">
         <v>0</v>
       </c>
       <c r="AC101" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD101" s="5">
         <v>0</v>
@@ -31118,7 +31136,7 @@
         <v>0</v>
       </c>
       <c r="AJ101" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
@@ -31137,13 +31155,13 @@
         <v>0</v>
       </c>
       <c r="F102" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G102" s="4">
         <v>0</v>
       </c>
       <c r="H102" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" s="3">
         <v>1</v>
@@ -31200,13 +31218,13 @@
         <v>0</v>
       </c>
       <c r="AA102" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB102" s="6">
         <v>0</v>
       </c>
       <c r="AC102" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD102" s="5">
         <v>0</v>
@@ -31227,7 +31245,7 @@
         <v>0</v>
       </c>
       <c r="AJ102" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
@@ -31246,13 +31264,13 @@
         <v>0</v>
       </c>
       <c r="F103" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103" s="4">
         <v>0</v>
       </c>
       <c r="H103" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" s="3">
         <v>0</v>
@@ -31309,13 +31327,13 @@
         <v>0</v>
       </c>
       <c r="AA103" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB103" s="6">
         <v>0</v>
       </c>
       <c r="AC103" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD103" s="5">
         <v>0</v>
@@ -31336,7 +31354,7 @@
         <v>0</v>
       </c>
       <c r="AJ103" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
@@ -31355,13 +31373,13 @@
         <v>0</v>
       </c>
       <c r="F104" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" s="4">
         <v>0</v>
       </c>
       <c r="H104" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" s="3">
         <v>0</v>
@@ -31418,13 +31436,13 @@
         <v>0</v>
       </c>
       <c r="AA104" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB104" s="6">
         <v>0</v>
       </c>
       <c r="AC104" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD104" s="5">
         <v>0</v>
@@ -31445,7 +31463,7 @@
         <v>0</v>
       </c>
       <c r="AJ104" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
@@ -31464,7 +31482,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="4">
         <v>0</v>
@@ -31500,7 +31518,7 @@
         <v>0</v>
       </c>
       <c r="R105" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S105" s="3">
         <v>0</v>
@@ -38325,6 +38343,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="A155:A158"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="A80:A92"/>
+    <mergeCell ref="A93:A105"/>
+    <mergeCell ref="A106:A133"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="A139:A145"/>
+    <mergeCell ref="A146:A151"/>
     <mergeCell ref="A68:A79"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A19"/>
@@ -38337,21 +38365,12 @@
     <mergeCell ref="A51:A55"/>
     <mergeCell ref="A56:A60"/>
     <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A155:A158"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A162:A165"/>
-    <mergeCell ref="A80:A92"/>
-    <mergeCell ref="A93:A105"/>
-    <mergeCell ref="A106:A133"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="A139:A145"/>
-    <mergeCell ref="A146:A151"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>